<commit_message>
draft Adrien version (with footnotes)
</commit_message>
<xml_diff>
--- a/xlsx/'folder' missing.xlsx
+++ b/xlsx/'folder' missing.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t xml:space="preserve">Global tax on millionaires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sharing half of global tax with low-income countries</t>
   </si>
   <si>
     <t xml:space="preserve">A maximum wealth limit of $10 billion
@@ -458,22 +461,22 @@
         <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>0.199541385518588</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.235407197992704</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.360022360990976</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.263509714054735</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.337874186541836</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.615258955195884</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -481,22 +484,22 @@
         <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0570432872770611</v>
+        <v>0.199541385518588</v>
       </c>
       <c r="C5" t="n">
-        <v>0.146714122769711</v>
+        <v>0.235407197992704</v>
       </c>
       <c r="D5" t="n">
-        <v>0.204610110362681</v>
+        <v>0.360022360990976</v>
       </c>
       <c r="E5" t="n">
-        <v>0.10849487286792</v>
+        <v>0.263509714054735</v>
       </c>
       <c r="F5" t="n">
-        <v>0.199799135689725</v>
+        <v>0.337874186541836</v>
       </c>
       <c r="G5" t="n">
-        <v>0.483956303867612</v>
+        <v>0.615258955195884</v>
       </c>
     </row>
     <row r="6">
@@ -504,22 +507,22 @@
         <v>11</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0575260463918615</v>
+        <v>0.0570432872770611</v>
       </c>
       <c r="C6" t="n">
-        <v>0.128434426580614</v>
+        <v>0.146714122769711</v>
       </c>
       <c r="D6" t="n">
-        <v>0.206406954597061</v>
+        <v>0.204610110362681</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0639947015928308</v>
+        <v>0.10849487286792</v>
       </c>
       <c r="F6" t="n">
-        <v>0.153454882094592</v>
+        <v>0.199799135689725</v>
       </c>
       <c r="G6" t="n">
-        <v>0.373485958136766</v>
+        <v>0.483956303867612</v>
       </c>
     </row>
     <row r="7">
@@ -527,21 +530,44 @@
         <v>12</v>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>0.0575260463918615</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>0.128434426580614</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>0.206406954597061</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>0.0639947015928308</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>0.153454882094592</v>
       </c>
       <c r="G7" t="n">
+        <v>0.373485958136766</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Scenarios with non-universal participation, AR6 data (useless)
</commit_message>
<xml_diff>
--- a/xlsx/'folder' missing.xlsx
+++ b/xlsx/'folder' missing.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -560,40 +560,46 @@
     <t xml:space="preserve">Uruguay</t>
   </si>
   <si>
+    <t xml:space="preserve">Uzbekistan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saint Vincent and the Grenadines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venezuela</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vietnam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vanuatu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samoa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yemen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Africa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zambia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zimbabwe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dem USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-Dem USA</t>
+  </si>
+  <si>
     <t xml:space="preserve">USA</t>
   </si>
   <si>
-    <t xml:space="preserve">Uzbekistan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saint Vincent and the Grenadines</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Venezuela</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vietnam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vanuatu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Samoa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yemen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South Africa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zambia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zimbabwe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">npv_over_gdp_gcs_adj</t>
+    <t xml:space="preserve">Soptimistic_gain_adj_over_gdp_2030</t>
   </si>
 </sst>
 </file>
@@ -1505,247 +1511,235 @@
       <c r="GK1" t="s">
         <v>192</v>
       </c>
+      <c r="GL1" t="s">
+        <v>193</v>
+      </c>
+      <c r="GM1" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B2" t="n">
-        <v>0.108887140444102</v>
+        <v>0.442607759855407</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0110037200275776</v>
+        <v>0.0363536571999655</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0247722041692448</v>
-      </c>
-      <c r="E2" t="n">
-        <v>-0.00208408490165956</v>
-      </c>
-      <c r="F2" t="n">
-        <v>-0.0262957510980746</v>
-      </c>
+        <v>0.034703609775288</v>
+      </c>
+      <c r="E2"/>
+      <c r="F2"/>
       <c r="G2" t="n">
-        <v>0.000255248017093437</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0146274963530393</v>
-      </c>
-      <c r="I2" t="n">
-        <v>-0.00952418752944953</v>
-      </c>
-      <c r="J2" t="n">
-        <v>-0.00525449072947456</v>
-      </c>
+        <v>0.0256863986529112</v>
+      </c>
+      <c r="I2"/>
+      <c r="J2"/>
       <c r="K2" t="n">
-        <v>-0.00554537937860059</v>
+        <v>-0.0116626134644162</v>
       </c>
       <c r="L2" t="n">
-        <v>0.00373739240756085</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>0.343442068257327</v>
+        <v>1.4709087207359</v>
       </c>
       <c r="N2" t="n">
-        <v>-0.0158046281183817</v>
+        <v>-0.0306372508031646</v>
       </c>
       <c r="O2" t="n">
-        <v>0.0329350095447564</v>
+        <v>0.12104285292686</v>
       </c>
       <c r="P2" t="n">
-        <v>0.0974198940777267</v>
+        <v>0.397682602404877</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.0337657519077931</v>
+        <v>0.122900124175341</v>
       </c>
       <c r="R2" t="n">
-        <v>0.00166723414742693</v>
-      </c>
-      <c r="S2" t="n">
-        <v>-0.0309891254547789</v>
-      </c>
-      <c r="T2" t="n">
-        <v>-0.00888657713454943</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="S2"/>
+      <c r="T2"/>
       <c r="U2" t="n">
-        <v>0.0017610414146476</v>
+        <v>0</v>
       </c>
       <c r="V2" t="n">
-        <v>0.000423852987262193</v>
+        <v>0</v>
       </c>
       <c r="W2" t="n">
-        <v>0.00686586432735748</v>
+        <v>0</v>
       </c>
       <c r="X2" t="n">
-        <v>0.00823296412303885</v>
+        <v>0</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.00356117720613319</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>-0.00468063008087869</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>-0.0414575793033487</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="Z2"/>
+      <c r="AA2"/>
       <c r="AB2" t="n">
-        <v>0.00570262228263466</v>
+        <v>0.0142264644065338</v>
       </c>
       <c r="AC2" t="n">
         <v>0</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.237095759943111</v>
+        <v>1.06289942058061</v>
       </c>
       <c r="AE2" t="n">
-        <v>-0.0114834960364887</v>
+        <v>-0.0218098754504761</v>
       </c>
       <c r="AF2" t="n">
-        <v>-0.00556052519036778</v>
-      </c>
-      <c r="AG2" t="n">
-        <v>-0.00321498607627463</v>
-      </c>
+        <v>-0.0109297623983196</v>
+      </c>
+      <c r="AG2"/>
       <c r="AH2" t="n">
         <v>0</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.0186761549707129</v>
+        <v>0.0699447047896936</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.0414741265533555</v>
+        <v>0.166924533875106</v>
       </c>
       <c r="AK2" t="n">
-        <v>0.183420517518215</v>
+        <v>0.83598408692024</v>
       </c>
       <c r="AL2" t="n">
-        <v>0.000648585276686194</v>
+        <v>0</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.00423475216064677</v>
+        <v>0</v>
       </c>
       <c r="AN2" t="n">
-        <v>0.048070706305962</v>
+        <v>0.184039347608431</v>
       </c>
       <c r="AO2" t="n">
-        <v>0.00608680265552369</v>
+        <v>0.00967565394739187</v>
       </c>
       <c r="AP2" t="n">
-        <v>0.00196742003781327</v>
+        <v>0</v>
       </c>
       <c r="AQ2" t="n">
-        <v>0.00674238718449077</v>
+        <v>0.000378398450013442</v>
       </c>
       <c r="AR2" t="n">
-        <v>-0.00249298808663389</v>
+        <v>-0.00642636942332954</v>
       </c>
       <c r="AS2" t="n">
-        <v>-0.0104473766066253</v>
+        <v>-0.0339079420262336</v>
       </c>
       <c r="AT2" t="n">
-        <v>-0.0059639251093458</v>
+        <v>-0.0125275397455969</v>
       </c>
       <c r="AU2" t="n">
-        <v>0.027593519197459</v>
+        <v>0.10046898710192</v>
       </c>
       <c r="AV2" t="n">
-        <v>0.00359427505225345</v>
+        <v>0</v>
       </c>
       <c r="AW2" t="n">
-        <v>-0.0026535317371019</v>
+        <v>-0.00629443676154853</v>
       </c>
       <c r="AX2" t="n">
-        <v>0.00194263976598783</v>
+        <v>0</v>
       </c>
       <c r="AY2" t="n">
         <v>0</v>
       </c>
       <c r="AZ2" t="n">
-        <v>0.00315987244374518</v>
+        <v>0</v>
       </c>
       <c r="BA2" t="n">
-        <v>0.00501535248972177</v>
+        <v>0.00611945496414839</v>
       </c>
       <c r="BB2" t="n">
-        <v>0.111804111805177</v>
+        <v>0.441877554415933</v>
       </c>
       <c r="BC2" t="n">
-        <v>-0.0022612845681537</v>
+        <v>-0.00520198258476762</v>
       </c>
       <c r="BD2" t="n">
-        <v>-0.0119345505859691</v>
+        <v>-0.0377241945038636</v>
       </c>
       <c r="BE2" t="n">
-        <v>0.108573402268301</v>
+        <v>0.435619187319076</v>
       </c>
       <c r="BF2" t="n">
-        <v>-0.00529013686845409</v>
+        <v>-0.0112525711859789</v>
       </c>
       <c r="BG2" t="n">
-        <v>0.0174945713251826</v>
+        <v>0.0285925010970675</v>
       </c>
       <c r="BH2" t="n">
-        <v>-0.00226710997139519</v>
+        <v>-0.00549881143792919</v>
       </c>
       <c r="BI2" t="n">
-        <v>0.0356077308993374</v>
+        <v>0.0600040226405731</v>
       </c>
       <c r="BJ2" t="n">
-        <v>0.00116154090122794</v>
+        <v>0</v>
       </c>
       <c r="BK2" t="n">
-        <v>-0.00304073981463449</v>
+        <v>-0.00722320759664687</v>
       </c>
       <c r="BL2" t="n">
-        <v>0.00865105243384666</v>
+        <v>0.00920144043933313</v>
       </c>
       <c r="BM2" t="n">
-        <v>0.0187050135989212</v>
+        <v>0.0613071884669687</v>
       </c>
       <c r="BN2" t="n">
-        <v>0.0549467739735356</v>
+        <v>0.206697427830322</v>
       </c>
       <c r="BO2" t="n">
-        <v>0.115439922876583</v>
+        <v>0.466268485014821</v>
       </c>
       <c r="BP2" t="n">
-        <v>0.137418448992341</v>
+        <v>0.556466144145017</v>
       </c>
       <c r="BQ2" t="n">
         <v>0</v>
       </c>
       <c r="BR2" t="n">
-        <v>0.00112702865813094</v>
+        <v>-0.00240428666241817</v>
       </c>
       <c r="BS2" t="n">
-        <v>0.00215229923404564</v>
+        <v>0</v>
       </c>
       <c r="BT2" t="n">
-        <v>0.0144290108757639</v>
+        <v>0.011063572316679</v>
       </c>
       <c r="BU2" t="n">
-        <v>0.00246200267508261</v>
+        <v>0</v>
       </c>
       <c r="BV2" t="n">
-        <v>0.042282128301971</v>
+        <v>0.0732534504730981</v>
       </c>
       <c r="BW2" t="n">
-        <v>-0.000317212064551087</v>
+        <v>-0.00770412686575331</v>
       </c>
       <c r="BX2" t="n">
-        <v>0.105555751739304</v>
+        <v>0.239818813414395</v>
       </c>
       <c r="BY2" t="n">
-        <v>-0.00283470010986426</v>
+        <v>-0.0159233152086035</v>
       </c>
       <c r="BZ2" t="n">
-        <v>0.0116251304406202</v>
+        <v>0.0107923373320534</v>
       </c>
       <c r="CA2" t="n">
-        <v>0.00975213489455363</v>
+        <v>0.0269657637302264</v>
       </c>
       <c r="CB2" t="n">
-        <v>-0.00395394012748461</v>
+        <v>-0.00843252236211339</v>
       </c>
       <c r="CC2" t="n">
         <v>0</v>
@@ -1753,337 +1747,301 @@
       <c r="CD2" t="n">
         <v>0</v>
       </c>
-      <c r="CE2" t="n">
-        <v>-0.00461846455600237</v>
-      </c>
-      <c r="CF2" t="n">
-        <v>-0.0115142522259332</v>
-      </c>
+      <c r="CE2"/>
+      <c r="CF2"/>
       <c r="CG2" t="n">
-        <v>-0.00341862898290177</v>
+        <v>-0.00801015730541485</v>
       </c>
       <c r="CH2" t="n">
-        <v>0.00440687561250563</v>
+        <v>0</v>
       </c>
       <c r="CI2" t="n">
-        <v>0.000666729721842782</v>
+        <v>0</v>
       </c>
       <c r="CJ2" t="n">
-        <v>-0.00210140811037177</v>
-      </c>
-      <c r="CK2" t="n">
-        <v>-0.005417411936934</v>
-      </c>
+        <v>-0.00703889615832972</v>
+      </c>
+      <c r="CK2"/>
       <c r="CL2" t="n">
-        <v>0.0308278940232411</v>
+        <v>0.110774487067026</v>
       </c>
       <c r="CM2" t="n">
-        <v>0.0262109058276016</v>
+        <v>0.0221046114216444</v>
       </c>
       <c r="CN2" t="n">
-        <v>0.0373710110887162</v>
+        <v>0.113640404369409</v>
       </c>
       <c r="CO2" t="n">
-        <v>0.103226931948861</v>
-      </c>
-      <c r="CP2" t="n">
-        <v>-0.00920944885274189</v>
-      </c>
+        <v>0.199528461102441</v>
+      </c>
+      <c r="CP2"/>
       <c r="CQ2" t="n">
-        <v>-0.0198309376553362</v>
-      </c>
-      <c r="CR2" t="n">
-        <v>-0.0525606113002829</v>
-      </c>
+        <v>-0.0359451846669731</v>
+      </c>
+      <c r="CR2"/>
       <c r="CS2" t="n">
-        <v>0.00950127731875283</v>
+        <v>0.0171256720666182</v>
       </c>
       <c r="CT2" t="n">
         <v>0</v>
       </c>
       <c r="CU2" t="n">
-        <v>0.124105891121539</v>
+        <v>0.50440643242093</v>
       </c>
       <c r="CV2" t="n">
         <v>0</v>
       </c>
       <c r="CW2" t="n">
-        <v>0.00187223506214237</v>
+        <v>0</v>
       </c>
       <c r="CX2"/>
       <c r="CY2" t="n">
-        <v>0.00484433102042086</v>
+        <v>0.0162633852633878</v>
       </c>
       <c r="CZ2" t="n">
-        <v>0.00864605952560958</v>
+        <v>0</v>
       </c>
       <c r="DA2" t="n">
-        <v>-0.00590479290331772</v>
+        <v>-0.0237662133450578</v>
       </c>
       <c r="DB2" t="n">
-        <v>-0.00505693787251562</v>
+        <v>-0.00989873175103032</v>
       </c>
       <c r="DC2" t="n">
-        <v>-0.00640530448724469</v>
+        <v>-0.0280415130012458</v>
       </c>
       <c r="DD2" t="n">
-        <v>0.0138975285565704</v>
+        <v>0.04349375032316</v>
       </c>
       <c r="DE2" t="n">
-        <v>0.0253544258824537</v>
+        <v>0.0540543683312584</v>
       </c>
       <c r="DF2" t="n">
-        <v>0.173497354783874</v>
-      </c>
-      <c r="DG2" t="n">
-        <v>-0.00836659333428446</v>
-      </c>
+        <v>0.702493908685207</v>
+      </c>
+      <c r="DG2"/>
       <c r="DH2" t="n">
-        <v>0.00164484910454923</v>
+        <v>0</v>
       </c>
       <c r="DI2" t="n">
         <v>0</v>
       </c>
       <c r="DJ2" t="n">
-        <v>0.00826886761890025</v>
+        <v>0</v>
       </c>
       <c r="DK2" t="n">
-        <v>0.0963839199504269</v>
+        <v>0.424785877035098</v>
       </c>
       <c r="DL2" t="n">
-        <v>-0.0276098937700174</v>
+        <v>-0.0514504791319278</v>
       </c>
       <c r="DM2" t="n">
-        <v>0.102861261344411</v>
+        <v>0.177521122890708</v>
       </c>
       <c r="DN2" t="n">
-        <v>0.00444272772482555</v>
+        <v>0</v>
       </c>
       <c r="DO2" t="n">
         <v>0</v>
       </c>
       <c r="DP2" t="n">
-        <v>0.0883300792077625</v>
+        <v>0.345603258832404</v>
       </c>
       <c r="DQ2" t="n">
-        <v>0.00895390783713398</v>
-      </c>
-      <c r="DR2" t="n">
-        <v>-0.00971767675920828</v>
-      </c>
+        <v>0.012554352502925</v>
+      </c>
+      <c r="DR2"/>
       <c r="DS2" t="n">
-        <v>0.219924017814895</v>
-      </c>
-      <c r="DT2" t="n">
-        <v>-0.00166324617576075</v>
-      </c>
+        <v>0.912860825052543</v>
+      </c>
+      <c r="DT2"/>
       <c r="DU2" t="n">
         <v>0</v>
       </c>
       <c r="DV2" t="n">
-        <v>0.151741366320894</v>
+        <v>0.714849617938332</v>
       </c>
       <c r="DW2" t="n">
-        <v>0.0160267384297097</v>
+        <v>0.0582353547092945</v>
       </c>
       <c r="DX2" t="n">
-        <v>0.0503867848445468</v>
+        <v>0.082041159510952</v>
       </c>
       <c r="DY2" t="n">
-        <v>-0.00495605572779548</v>
+        <v>-0.0106723678437547</v>
       </c>
       <c r="DZ2" t="n">
-        <v>-0.00295065687140861</v>
+        <v>-0.00645138847787756</v>
       </c>
       <c r="EA2" t="n">
-        <v>0.0457772113272712</v>
+        <v>0.170288272515342</v>
       </c>
       <c r="EB2" t="n">
         <v>0</v>
       </c>
       <c r="EC2" t="n">
-        <v>-0.00150289017400864</v>
-      </c>
-      <c r="ED2" t="n">
-        <v>-0.0259486091973192</v>
-      </c>
+        <v>-0.00403775267183949</v>
+      </c>
+      <c r="ED2"/>
       <c r="EE2" t="n">
-        <v>0.0237635950162155</v>
-      </c>
-      <c r="EF2" t="n">
-        <v>-0.00387443803641743</v>
-      </c>
+        <v>0.0965625495302393</v>
+      </c>
+      <c r="EF2"/>
       <c r="EG2" t="n">
-        <v>0.0046432126726209</v>
+        <v>0</v>
       </c>
       <c r="EH2" t="n">
-        <v>0.0240970778635434</v>
-      </c>
-      <c r="EI2" t="n">
-        <v>-0.0296927948507129</v>
-      </c>
+        <v>0.0385582353552717</v>
+      </c>
+      <c r="EI2"/>
       <c r="EJ2" t="n">
-        <v>0.0503101436901928</v>
+        <v>0.093229198535131</v>
       </c>
       <c r="EK2" t="n">
-        <v>-0.00525085882094427</v>
+        <v>-0.0233160180060687</v>
       </c>
       <c r="EL2" t="n">
-        <v>0.145568354353361</v>
+        <v>0.427363521268592</v>
       </c>
       <c r="EM2" t="n">
-        <v>-0.000141700520967292</v>
+        <v>-0.00237631977058196</v>
       </c>
       <c r="EN2" t="n">
-        <v>0.00509649178924633</v>
+        <v>0</v>
       </c>
       <c r="EO2" t="n">
-        <v>0.028961237803318</v>
-      </c>
-      <c r="EP2" t="n">
-        <v>-0.0242531405012455</v>
-      </c>
+        <v>0.103922639150555</v>
+      </c>
+      <c r="EP2"/>
       <c r="EQ2" t="n">
-        <v>0.00236816135539102</v>
-      </c>
-      <c r="ER2" t="n">
-        <v>-0.00386889030674031</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="ER2"/>
       <c r="ES2" t="n">
-        <v>0.0993101247995003</v>
-      </c>
-      <c r="ET2" t="n">
-        <v>-0.0431847809177645</v>
-      </c>
+        <v>0.397774447916352</v>
+      </c>
+      <c r="ET2"/>
       <c r="EU2" t="n">
-        <v>0.0520317535427039</v>
+        <v>0.196251455354028</v>
       </c>
       <c r="EV2" t="n">
-        <v>0.0052037134890277</v>
-      </c>
-      <c r="EW2" t="n">
-        <v>-0.0237434999889371</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="EW2"/>
       <c r="EX2" t="n">
-        <v>0.0657086142192976</v>
+        <v>0.133783254435204</v>
       </c>
       <c r="EY2" t="n">
-        <v>0.144017977302937</v>
+        <v>0.572657174465654</v>
       </c>
       <c r="EZ2" t="n">
-        <v>0.0170939664796153</v>
+        <v>0.0151096473898082</v>
       </c>
       <c r="FA2" t="n">
-        <v>0.210902537742548</v>
+        <v>0.951619693117974</v>
       </c>
       <c r="FB2" t="n">
-        <v>0.00172353646468634</v>
+        <v>0</v>
       </c>
       <c r="FC2" t="n">
-        <v>0.26761587991902</v>
+        <v>0.97992583675477</v>
       </c>
       <c r="FD2" t="n">
-        <v>0.0246532076990458</v>
+        <v>0.0867064489873992</v>
       </c>
       <c r="FE2" t="n">
-        <v>0.00180075630074131</v>
+        <v>0</v>
       </c>
       <c r="FF2" t="n">
-        <v>-0.00550656675219813</v>
+        <v>-0.0210040337213707</v>
       </c>
       <c r="FG2" t="n">
-        <v>-0.00780376304943126</v>
+        <v>-0.0254741140578765</v>
       </c>
       <c r="FH2" t="n">
-        <v>-0.00182518149622324</v>
+        <v>-0.00448931863020271</v>
       </c>
       <c r="FI2" t="n">
-        <v>0.00440519145534735</v>
-      </c>
-      <c r="FJ2" t="n">
-        <v>-0.0162638592479343</v>
-      </c>
+        <v>0.00613231900291519</v>
+      </c>
+      <c r="FJ2"/>
       <c r="FK2" t="n">
-        <v>0.0805769695089553</v>
+        <v>0.274290325231816</v>
       </c>
       <c r="FL2" t="n">
-        <v>0.124337663713821</v>
+        <v>0.561155004743766</v>
       </c>
       <c r="FM2" t="n">
-        <v>0.0148634649208408</v>
+        <v>0</v>
       </c>
       <c r="FN2" t="n">
-        <v>0.0000586530168694682</v>
+        <v>0</v>
       </c>
       <c r="FO2" t="n">
-        <v>0.0622606858098577</v>
-      </c>
-      <c r="FP2" t="n">
-        <v>-0.000887332559606418</v>
-      </c>
+        <v>0.149096837497506</v>
+      </c>
+      <c r="FP2"/>
       <c r="FQ2" t="n">
-        <v>0.0990471954841045</v>
+        <v>0.184878674715778</v>
       </c>
       <c r="FR2" t="n">
-        <v>0.0174410856399936</v>
-      </c>
-      <c r="FS2" t="n">
-        <v>-0.0400209118736685</v>
-      </c>
+        <v>0.0291827994614112</v>
+      </c>
+      <c r="FS2"/>
       <c r="FT2" t="n">
-        <v>0.00891633228056771</v>
+        <v>0.0238281065389928</v>
       </c>
       <c r="FU2" t="n">
-        <v>0.000977374717971643</v>
+        <v>0</v>
       </c>
       <c r="FV2" t="n">
-        <v>0.034165572580637</v>
+        <v>0.0645946780307104</v>
       </c>
       <c r="FW2" t="n">
-        <v>0.06496342863736</v>
+        <v>0.269052124065286</v>
       </c>
       <c r="FX2" t="n">
-        <v>0.0870377353006256</v>
+        <v>0.360758420250027</v>
       </c>
       <c r="FY2" t="n">
-        <v>0.00367442186187241</v>
-      </c>
-      <c r="FZ2" t="n">
-        <v>-0.000802031089572651</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="FZ2"/>
       <c r="GA2" t="n">
-        <v>-0.0121582890723282</v>
+        <v>0</v>
       </c>
       <c r="GB2" t="n">
-        <v>0.00445101787348296</v>
+        <v>0</v>
       </c>
       <c r="GC2" t="n">
-        <v>0.00383780040653276</v>
+        <v>0.0972200902726076</v>
       </c>
       <c r="GD2" t="n">
-        <v>0.0443895360951264</v>
+        <v>0.0733079630670761</v>
       </c>
       <c r="GE2" t="n">
-        <v>0.0243411413378213</v>
+        <v>0.0984667030473454</v>
       </c>
       <c r="GF2" t="n">
-        <v>0.0489199648899973</v>
+        <v>0.0374017235368603</v>
       </c>
       <c r="GG2" t="n">
-        <v>0.0204816697927513</v>
+        <v>0.58046366968681</v>
       </c>
       <c r="GH2" t="n">
-        <v>0.162481572939206</v>
+        <v>0</v>
       </c>
       <c r="GI2" t="n">
-        <v>0</v>
+        <v>0.145663151967098</v>
       </c>
       <c r="GJ2" t="n">
-        <v>0.037785744105228</v>
+        <v>0.0473984698509576</v>
       </c>
       <c r="GK2" t="n">
-        <v>0.0176333705733482</v>
-      </c>
+        <v>-0.00990695992677429</v>
+      </c>
+      <c r="GL2"/>
+      <c r="GM2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add data missing countries (TWN, SSD, SWZ, PRK)
</commit_message>
<xml_diff>
--- a/xlsx/'folder' missing.xlsx
+++ b/xlsx/'folder' missing.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="177">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -446,6 +446,9 @@
     <t xml:space="preserve">Serbia</t>
   </si>
   <si>
+    <t xml:space="preserve">South Sudan</t>
+  </si>
+  <si>
     <t xml:space="preserve">Suriname</t>
   </si>
   <si>
@@ -458,7 +461,7 @@
     <t xml:space="preserve">Sweden</t>
   </si>
   <si>
-    <t xml:space="preserve">Eswatini</t>
+    <t xml:space="preserve">Swaziland</t>
   </si>
   <si>
     <t xml:space="preserve">Syria</t>
@@ -491,6 +494,9 @@
     <t xml:space="preserve">Turkey</t>
   </si>
   <si>
+    <t xml:space="preserve">Taiwan</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tanzania</t>
   </si>
   <si>
@@ -531,6 +537,9 @@
   </si>
   <si>
     <t xml:space="preserve">Zimbabwe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Korea</t>
   </si>
   <si>
     <t xml:space="preserve">npv_over_gdp_gcs_adj</t>
@@ -1385,61 +1394,70 @@
       <c r="FQ1" t="s">
         <v>172</v>
       </c>
+      <c r="FR1" t="s">
+        <v>173</v>
+      </c>
+      <c r="FS1" t="s">
+        <v>174</v>
+      </c>
+      <c r="FT1" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0473115544403191</v>
+        <v>0.0356875191410064</v>
       </c>
       <c r="C2" t="n">
-        <v>0.027683098944982</v>
+        <v>0.0245093245453326</v>
       </c>
       <c r="D2" t="n">
-        <v>0.00646933050295286</v>
+        <v>0.00485902340826297</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.0209684670020598</v>
+        <v>-0.0192670547030884</v>
       </c>
       <c r="F2" t="n">
-        <v>0.000845951004653832</v>
+        <v>0.00108512899450586</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0060239720279802</v>
+        <v>0.00449424818629026</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.021422938153989</v>
+        <v>-0.0195639231891367</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.00627333734947143</v>
+        <v>-0.00596032831881557</v>
       </c>
       <c r="J2" t="n">
-        <v>0.00321366432749366</v>
+        <v>0.0032536988768513</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0691716690881289</v>
+        <v>0.0483747658269906</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.00834471896408628</v>
+        <v>-0.00789080659297457</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0312608822758166</v>
+        <v>0.0212675033974482</v>
       </c>
       <c r="N2" t="n">
-        <v>0.0471365439020625</v>
+        <v>0.0342776155554819</v>
       </c>
       <c r="O2" t="n">
-        <v>0.0248557634924505</v>
+        <v>0.0188932931639619</v>
       </c>
       <c r="P2" t="n">
-        <v>-0.00340490904291284</v>
+        <v>-0.00357872757948836</v>
       </c>
       <c r="Q2" t="n">
-        <v>-0.0307593821874734</v>
+        <v>-0.028050563280491</v>
       </c>
       <c r="R2" t="n">
-        <v>0.000263419289630564</v>
+        <v>0.000948396869510171</v>
       </c>
       <c r="S2" t="n">
         <v>0</v>
@@ -1448,169 +1466,169 @@
         <v>0</v>
       </c>
       <c r="U2" t="n">
-        <v>0.011505453388521</v>
+        <v>0.00935424148242623</v>
       </c>
       <c r="V2" t="n">
-        <v>0.00582319732688445</v>
+        <v>0.00440499697238454</v>
       </c>
       <c r="W2" t="n">
-        <v>0.00361116196041247</v>
+        <v>0.00332627429809869</v>
       </c>
       <c r="X2" t="n">
-        <v>0.00247852247707509</v>
+        <v>0.00303748194340396</v>
       </c>
       <c r="Y2" t="n">
-        <v>-0.0116051101941872</v>
+        <v>-0.00940032780937369</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.00363033466706034</v>
+        <v>0.00259078284405133</v>
       </c>
       <c r="AA2" t="n">
         <v>0</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.0998253684115784</v>
+        <v>0.0720853751182868</v>
       </c>
       <c r="AC2" t="n">
-        <v>-0.0196663799525681</v>
+        <v>-0.0174662344061285</v>
       </c>
       <c r="AD2" t="n">
-        <v>-0.00171942325381162</v>
+        <v>-0.00168903634032235</v>
       </c>
       <c r="AE2" t="n">
-        <v>-0.000737240603796377</v>
+        <v>-0.000452751125956252</v>
       </c>
       <c r="AF2" t="n">
         <v>0</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.00655666101581609</v>
+        <v>0.00381108654538279</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.0200587751132735</v>
+        <v>0.0141145555006051</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.0388801081666401</v>
+        <v>0.0267719634217861</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.0177142228090692</v>
+        <v>0.0134779986074219</v>
       </c>
       <c r="AK2" t="n">
-        <v>0.00679895884989255</v>
+        <v>0.00552328418156858</v>
       </c>
       <c r="AL2" t="n">
-        <v>0.0225605146388077</v>
+        <v>0.0157497236895028</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.011475913029326</v>
+        <v>0.00822445907053969</v>
       </c>
       <c r="AN2" t="n">
-        <v>0.00638947205078423</v>
+        <v>0.00526921534587604</v>
       </c>
       <c r="AO2" t="n">
-        <v>0.00528540475597671</v>
+        <v>0.00471382247896825</v>
       </c>
       <c r="AP2" t="n">
         <v>0</v>
       </c>
       <c r="AQ2" t="n">
-        <v>-0.0149742989951371</v>
+        <v>-0.0139657077075483</v>
       </c>
       <c r="AR2" t="n">
-        <v>-0.00975019897784493</v>
+        <v>-0.00911783350691932</v>
       </c>
       <c r="AS2" t="n">
-        <v>0.0149277541082539</v>
+        <v>0.0097576341144787</v>
       </c>
       <c r="AT2" t="n">
-        <v>-0.00345948018453657</v>
+        <v>-0.00339776498715599</v>
       </c>
       <c r="AU2" t="n">
-        <v>0.00684484228623837</v>
+        <v>0.00553805759636965</v>
       </c>
       <c r="AV2" t="n">
         <v>0</v>
       </c>
       <c r="AW2" t="n">
-        <v>0.00416965907212757</v>
+        <v>0.00354576237831884</v>
       </c>
       <c r="AX2" t="n">
-        <v>0.0000655412854622844</v>
+        <v>0</v>
       </c>
       <c r="AY2" t="n">
-        <v>0.0545116067121763</v>
+        <v>0.0386959335978544</v>
       </c>
       <c r="AZ2" t="n">
-        <v>-0.000341854778693429</v>
+        <v>-0.000175342219450234</v>
       </c>
       <c r="BA2" t="n">
-        <v>-0.0299755706625139</v>
+        <v>-0.0274994598051434</v>
       </c>
       <c r="BB2" t="n">
-        <v>0.0478987255873311</v>
+        <v>0.0343323336334576</v>
       </c>
       <c r="BC2" t="n">
-        <v>-0.00701861429322501</v>
+        <v>-0.00641204888385086</v>
       </c>
       <c r="BD2" t="n">
-        <v>0.0146913855811081</v>
+        <v>0.0114080130803961</v>
       </c>
       <c r="BE2" t="n">
-        <v>-0.00236664949364971</v>
+        <v>-0.00215723629597085</v>
       </c>
       <c r="BF2" t="n">
-        <v>0.000598972099262507</v>
+        <v>0.00027259568638115</v>
       </c>
       <c r="BG2" t="n">
-        <v>-0.00391023724708056</v>
+        <v>-0.00361932923857326</v>
       </c>
       <c r="BH2" t="n">
-        <v>0.00155695708816377</v>
+        <v>0.000864284087766568</v>
       </c>
       <c r="BI2" t="n">
-        <v>0.0136048428381538</v>
+        <v>0.00978622874234512</v>
       </c>
       <c r="BJ2" t="n">
-        <v>0.0120017027501727</v>
+        <v>0.00782774561651669</v>
       </c>
       <c r="BK2" t="n">
-        <v>0.0374154706795202</v>
+        <v>0.0277495643509862</v>
       </c>
       <c r="BL2" t="n">
-        <v>0.0346284118700587</v>
+        <v>0.0237829750424552</v>
       </c>
       <c r="BM2" t="n">
-        <v>0.000656068583580235</v>
+        <v>0.00087514199821241</v>
       </c>
       <c r="BN2" t="n">
-        <v>-0.000159118901403247</v>
+        <v>-0.0000456385848944426</v>
       </c>
       <c r="BO2" t="n">
-        <v>0.0111445599922747</v>
+        <v>0.0084903254931292</v>
       </c>
       <c r="BP2" t="n">
-        <v>0.00197901173587301</v>
+        <v>0.00195197825112725</v>
       </c>
       <c r="BQ2" t="n">
-        <v>0.0184660043330005</v>
+        <v>0.0141076548899157</v>
       </c>
       <c r="BR2" t="n">
-        <v>0.0000323976781954318</v>
+        <v>0</v>
       </c>
       <c r="BS2" t="n">
-        <v>0.0356377792913219</v>
+        <v>0.0251736522365122</v>
       </c>
       <c r="BT2" t="n">
-        <v>-0.0022091155208913</v>
+        <v>-0.00231476456003901</v>
       </c>
       <c r="BU2" t="n">
-        <v>0.00553261904391908</v>
+        <v>0.00417653419895301</v>
       </c>
       <c r="BV2" t="n">
-        <v>0.0102813784061415</v>
+        <v>0.00791721275666003</v>
       </c>
       <c r="BW2" t="n">
-        <v>-0.00495643798904049</v>
+        <v>-0.00478115517446086</v>
       </c>
       <c r="BX2" t="n">
         <v>0</v>
@@ -1619,292 +1637,301 @@
         <v>0</v>
       </c>
       <c r="BZ2" t="n">
-        <v>-0.0118571139391708</v>
+        <v>-0.0111873316964491</v>
       </c>
       <c r="CA2" t="n">
-        <v>-0.000176194117031815</v>
+        <v>-0.0000425842361025672</v>
       </c>
       <c r="CB2" t="n">
-        <v>-0.00200566218562204</v>
+        <v>-0.00168739076673791</v>
       </c>
       <c r="CC2" t="n">
-        <v>0.0138873531678787</v>
+        <v>0.0119701379252103</v>
       </c>
       <c r="CD2" t="n">
-        <v>0.0000803365308710959</v>
+        <v>0</v>
       </c>
       <c r="CE2" t="n">
-        <v>-0.008174034575885</v>
+        <v>-0.00681428756912262</v>
       </c>
       <c r="CF2" t="n">
-        <v>-0.0230297942818188</v>
+        <v>-0.0185156790422546</v>
       </c>
       <c r="CG2" t="n">
-        <v>0.0281169615568363</v>
+        <v>0.020479930717612</v>
       </c>
       <c r="CH2" t="n">
-        <v>0.00644377449918904</v>
+        <v>0.00378719029399407</v>
       </c>
       <c r="CI2" t="n">
-        <v>0.0195205785875397</v>
+        <v>0.0143844156650474</v>
       </c>
       <c r="CJ2" t="n">
-        <v>-0.00671418159062439</v>
+        <v>-0.00553352163372765</v>
       </c>
       <c r="CK2" t="n">
-        <v>-0.0374502329731794</v>
+        <v>-0.0336755245683259</v>
       </c>
       <c r="CL2" t="n">
-        <v>0.0121084774343685</v>
+        <v>0.00921245988178436</v>
       </c>
       <c r="CM2" t="n">
-        <v>0.0000119411901955365</v>
+        <v>0</v>
       </c>
       <c r="CN2" t="n">
-        <v>0.0451749826657626</v>
+        <v>0.0298767366239188</v>
       </c>
       <c r="CO2" t="n">
         <v>0</v>
       </c>
       <c r="CP2" t="n">
-        <v>0.00750125190389791</v>
+        <v>0.00601780172410653</v>
       </c>
       <c r="CQ2" t="n">
-        <v>0.00796599713507144</v>
+        <v>0.00422090096016206</v>
       </c>
       <c r="CR2" t="n">
-        <v>-0.00285205567296823</v>
+        <v>-0.0026577546000342</v>
       </c>
       <c r="CS2" t="n">
-        <v>-0.00994488041388503</v>
+        <v>-0.00930710478481006</v>
       </c>
       <c r="CT2" t="n">
-        <v>-0.000890832078768026</v>
+        <v>-0.000949689490165741</v>
       </c>
       <c r="CU2" t="n">
-        <v>0.00114833054464046</v>
+        <v>0.000402191926225262</v>
       </c>
       <c r="CV2" t="n">
-        <v>0.00115738795961354</v>
+        <v>0.000369642433183947</v>
       </c>
       <c r="CW2" t="n">
-        <v>0.0442854112053684</v>
+        <v>0.0311679581683741</v>
       </c>
       <c r="CX2" t="n">
-        <v>0.00671788964808634</v>
+        <v>0.0055971138226317</v>
       </c>
       <c r="CY2" t="n">
-        <v>0.000745194808669985</v>
+        <v>0.000941290671386018</v>
       </c>
       <c r="CZ2" t="n">
         <v>0</v>
       </c>
       <c r="DA2" t="n">
-        <v>0.0262319943760962</v>
+        <v>0.0186058210254922</v>
       </c>
       <c r="DB2" t="n">
-        <v>-0.00233255307046466</v>
+        <v>-0.00227375956591908</v>
       </c>
       <c r="DC2" t="n">
-        <v>0.028698970876484</v>
+        <v>0.0234979287060741</v>
       </c>
       <c r="DD2" t="n">
         <v>0</v>
       </c>
       <c r="DE2" t="n">
-        <v>-0.00215691474097922</v>
+        <v>-0.0023201591927836</v>
       </c>
       <c r="DF2" t="n">
-        <v>0.0397685017923518</v>
+        <v>0.0270156792832291</v>
       </c>
       <c r="DG2" t="n">
-        <v>0.0195734633552438</v>
+        <v>0.0136939480038112</v>
       </c>
       <c r="DH2" t="n">
-        <v>-0.000341767897087424</v>
+        <v>-0.000493770695573336</v>
       </c>
       <c r="DI2" t="n">
-        <v>0.0709809793256854</v>
+        <v>0.0507055324246146</v>
       </c>
       <c r="DJ2" t="n">
-        <v>-0.00188947875362367</v>
+        <v>-0.00165267414881285</v>
       </c>
       <c r="DK2" t="n">
-        <v>0.00139635063055405</v>
+        <v>0.000710620443974512</v>
       </c>
       <c r="DL2" t="n">
-        <v>0.0727056835303598</v>
+        <v>0.0508260395287347</v>
       </c>
       <c r="DM2" t="n">
-        <v>0.0126872854615296</v>
+        <v>0.00905537616689578</v>
       </c>
       <c r="DN2" t="n">
-        <v>0.0110579455530388</v>
+        <v>0.00790150701364007</v>
       </c>
       <c r="DO2" t="n">
-        <v>-0.00975527683276491</v>
+        <v>-0.0091759707073975</v>
       </c>
       <c r="DP2" t="n">
-        <v>-0.00590987865005575</v>
+        <v>-0.00542917202585966</v>
       </c>
       <c r="DQ2" t="n">
-        <v>0.0369484387288584</v>
+        <v>0.0272860223193478</v>
       </c>
       <c r="DR2" t="n">
-        <v>-0.00613163583315443</v>
+        <v>-0.00547607191617818</v>
       </c>
       <c r="DS2" t="n">
-        <v>-0.0167866267135453</v>
+        <v>-0.0128877588171232</v>
       </c>
       <c r="DT2" t="n">
-        <v>0.0187436424570455</v>
+        <v>0.0143211983784643</v>
       </c>
       <c r="DU2" t="n">
-        <v>0.000301727492352522</v>
+        <v>0.000225967467783011</v>
       </c>
       <c r="DV2" t="n">
-        <v>0.00198877354217597</v>
+        <v>0.00159986770542296</v>
       </c>
       <c r="DW2" t="n">
-        <v>0.01893766787156</v>
+        <v>0.0150041297271365</v>
       </c>
       <c r="DX2" t="n">
-        <v>0.0276252169021498</v>
+        <v>0.0207380247279573</v>
       </c>
       <c r="DY2" t="n">
-        <v>-0.00878349380015038</v>
+        <v>-0.00753370610178701</v>
       </c>
       <c r="DZ2" t="n">
-        <v>-0.000160226683455865</v>
+        <v>-0.0000663916710112407</v>
       </c>
       <c r="EA2" t="n">
-        <v>0.00735731044043458</v>
+        <v>0.00540535486818598</v>
       </c>
       <c r="EB2" t="n">
-        <v>-0.0337191883031047</v>
+        <v>-0.03061972379237</v>
       </c>
       <c r="EC2" t="n">
-        <v>-0.00129305244918867</v>
+        <v>-0.00146784459846493</v>
       </c>
       <c r="ED2" t="n">
-        <v>-0.0103399018676428</v>
+        <v>-0.00883457882085307</v>
       </c>
       <c r="EE2" t="n">
-        <v>0.044810091189074</v>
+        <v>0.0333759824518872</v>
       </c>
       <c r="EF2" t="n">
-        <v>-0.0248052138753236</v>
+        <v>-0.0223352267104535</v>
       </c>
       <c r="EG2" t="n">
-        <v>0.0106411551954263</v>
+        <v>0.00710597632312938</v>
       </c>
       <c r="EH2" t="n">
-        <v>0.018918543128615</v>
+        <v>0.0129364504028897</v>
       </c>
       <c r="EI2" t="n">
-        <v>-0.00444368848834366</v>
+        <v>-0.00343989285860491</v>
       </c>
       <c r="EJ2" t="n">
-        <v>0.0564146370863929</v>
+        <v>0.043602115956949</v>
       </c>
       <c r="EK2" t="n">
-        <v>0.0519096981370061</v>
+        <v>0.0368949834078866</v>
       </c>
       <c r="EL2" t="n">
-        <v>0.0156285713710293</v>
+        <v>0.0126714808434525</v>
       </c>
       <c r="EM2" t="n">
-        <v>0.023762367047538</v>
+        <v>0.0157160393620034</v>
       </c>
       <c r="EN2" t="n">
         <v>0</v>
       </c>
       <c r="EO2" t="n">
-        <v>0.000612027441181282</v>
+        <v>0.0184514599384831</v>
       </c>
       <c r="EP2" t="n">
-        <v>-0.00717363514901583</v>
+        <v>0.000753019804966783</v>
       </c>
       <c r="EQ2" t="n">
-        <v>-0.00369549574481091</v>
+        <v>-0.00671190374929643</v>
       </c>
       <c r="ER2" t="n">
-        <v>-0.00197832501337339</v>
+        <v>-0.00313607806484724</v>
       </c>
       <c r="ES2" t="n">
-        <v>0.0086647071572602</v>
+        <v>-0.00188860615536026</v>
       </c>
       <c r="ET2" t="n">
-        <v>0.000556530172233543</v>
+        <v>0.00612973875503128</v>
       </c>
       <c r="EU2" t="n">
-        <v>0.0520947340267544</v>
+        <v>0.0000736262607416137</v>
       </c>
       <c r="EV2" t="n">
-        <v>0.0356922101279335</v>
+        <v>0.0379975293287518</v>
       </c>
       <c r="EW2" t="n">
-        <v>0.000385974513226746</v>
+        <v>0.0238117068840801</v>
       </c>
       <c r="EX2" t="n">
-        <v>0.0219852684326196</v>
+        <v>0.000105141673696271</v>
       </c>
       <c r="EY2" t="n">
-        <v>-0.0200436972802212</v>
+        <v>0.0166224737730836</v>
       </c>
       <c r="EZ2" t="n">
-        <v>0.0120279326867949</v>
+        <v>-0.0184272232164803</v>
       </c>
       <c r="FA2" t="n">
-        <v>-0.0581328338828642</v>
+        <v>0.00893013741790224</v>
       </c>
       <c r="FB2" t="n">
-        <v>0.000334845649985921</v>
+        <v>-0.0477331772302383</v>
       </c>
       <c r="FC2" t="n">
-        <v>-0.00338209086750734</v>
+        <v>0.0000395077307772004</v>
       </c>
       <c r="FD2" t="n">
-        <v>0.0283667379035772</v>
+        <v>-0.00325575873096219</v>
       </c>
       <c r="FE2" t="n">
-        <v>0.0386024456351803</v>
+        <v>-0.00361399040331989</v>
       </c>
       <c r="FF2" t="n">
+        <v>0.0207913883145536</v>
+      </c>
+      <c r="FG2" t="n">
+        <v>0.0281358634225232</v>
+      </c>
+      <c r="FH2" t="n">
         <v>0</v>
       </c>
-      <c r="FG2" t="n">
-        <v>0.00143525891932353</v>
-      </c>
-      <c r="FH2" t="n">
-        <v>-0.019200629817618</v>
-      </c>
       <c r="FI2" t="n">
-        <v>0.00000725359318094457</v>
+        <v>0.00109782220453865</v>
       </c>
       <c r="FJ2" t="n">
-        <v>0.00190375512491479</v>
+        <v>-0.0180946978367277</v>
       </c>
       <c r="FK2" t="n">
-        <v>0.00309717584488171</v>
+        <v>0</v>
       </c>
       <c r="FL2" t="n">
-        <v>0.0440512309544695</v>
+        <v>0.00237970218824875</v>
       </c>
       <c r="FM2" t="n">
-        <v>0.0234884725315612</v>
+        <v>0.00191744912894136</v>
       </c>
       <c r="FN2" t="n">
-        <v>0.0143529476603696</v>
+        <v>0.0337649851889989</v>
       </c>
       <c r="FO2" t="n">
+        <v>0.0189125984800407</v>
+      </c>
+      <c r="FP2" t="n">
+        <v>0.00916881990959784</v>
+      </c>
+      <c r="FQ2" t="n">
         <v>0</v>
       </c>
-      <c r="FP2" t="n">
-        <v>0.0164629136836297</v>
-      </c>
-      <c r="FQ2" t="n">
-        <v>0.00661848062256457</v>
+      <c r="FR2" t="n">
+        <v>0.0117674259759046</v>
+      </c>
+      <c r="FS2" t="n">
+        <v>0.00319430573264842</v>
+      </c>
+      <c r="FT2" t="n">
+        <v>0.0789934738013299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix bug Dem USA
</commit_message>
<xml_diff>
--- a/xlsx/'folder' missing.xlsx
+++ b/xlsx/'folder' missing.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="178">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -218,6 +218,9 @@
     <t xml:space="preserve">Guyana</t>
   </si>
   <si>
+    <t xml:space="preserve">Hong Kong</t>
+  </si>
+  <si>
     <t xml:space="preserve">Honduras</t>
   </si>
   <si>
@@ -542,7 +545,7 @@
     <t xml:space="preserve">North Korea</t>
   </si>
   <si>
-    <t xml:space="preserve">npv_pa_gcs_adj</t>
+    <t xml:space="preserve">Scentral_npv_over_gdp_gcs_adj</t>
   </si>
 </sst>
 </file>
@@ -1403,535 +1406,489 @@
       <c r="FT1" t="s">
         <v>175</v>
       </c>
+      <c r="FU1" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B2" t="n">
-        <v>16724.3199939839</v>
+        <v>0.0181978479454534</v>
       </c>
       <c r="C2" t="n">
-        <v>13170.7571451773</v>
+        <v>0.00605031278738703</v>
       </c>
       <c r="D2" t="n">
-        <v>7264.42780919361</v>
-      </c>
-      <c r="E2" t="n">
-        <v>-74107.7710489145</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E2"/>
       <c r="F2" t="n">
-        <v>796.657555273694</v>
+        <v>0.000478969338267119</v>
       </c>
       <c r="G2" t="n">
-        <v>7558.03206796017</v>
-      </c>
-      <c r="H2" t="n">
-        <v>-37993.3332164902</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H2"/>
       <c r="I2" t="n">
-        <v>-11943.9327837908</v>
+        <v>-0.00865528391275657</v>
       </c>
       <c r="J2" t="n">
-        <v>6309.53549918239</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>17616.475027131</v>
+        <v>0.023278051478139</v>
       </c>
       <c r="L2" t="n">
-        <v>-16422.772940337</v>
+        <v>-0.0106350667875789</v>
       </c>
       <c r="M2" t="n">
-        <v>12050.2459221737</v>
+        <v>0.0046695949530543</v>
       </c>
       <c r="N2" t="n">
-        <v>16600.4157220683</v>
+        <v>0.0150994491515351</v>
       </c>
       <c r="O2" t="n">
-        <v>15720.2695896445</v>
+        <v>0.00885096520762095</v>
       </c>
       <c r="P2" t="n">
-        <v>-13976.7262552672</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>-91237.2766895412</v>
-      </c>
+        <v>-0.0045165510205679</v>
+      </c>
+      <c r="Q2"/>
       <c r="R2" t="n">
-        <v>6117.14893564724</v>
+        <v>0.000359472231601866</v>
       </c>
       <c r="S2" t="n">
-        <v>-13669.2046552423</v>
+        <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>-2675.8152520416</v>
+        <v>0</v>
       </c>
       <c r="U2" t="n">
-        <v>11089.0705415183</v>
+        <v>0.0013842547654194</v>
       </c>
       <c r="V2" t="n">
-        <v>7800.57342508217</v>
+        <v>0.000741413449639804</v>
       </c>
       <c r="W2" t="n">
-        <v>7323.1244689596</v>
+        <v>0.000608722598182665</v>
       </c>
       <c r="X2" t="n">
-        <v>5152.41681144098</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>-21441.6908363384</v>
-      </c>
+        <v>0.000971757976059452</v>
+      </c>
+      <c r="Y2"/>
       <c r="Z2" t="n">
-        <v>7287.87771481083</v>
+        <v>0</v>
       </c>
       <c r="AA2" t="n">
-        <v>-5008.53048842689</v>
+        <v>0</v>
       </c>
       <c r="AB2" t="n">
-        <v>16986.7716741738</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>-35245.1732967335</v>
-      </c>
+        <v>0.0329172745649323</v>
+      </c>
+      <c r="AC2"/>
       <c r="AD2" t="n">
-        <v>-788.904111363773</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>-1328.83260749747</v>
-      </c>
+        <v>-0.00349480425447978</v>
+      </c>
+      <c r="AE2"/>
       <c r="AF2" t="n">
-        <v>-1650.48578246452</v>
+        <v>0</v>
       </c>
       <c r="AG2" t="n">
-        <v>7588.32953445467</v>
+        <v>0.000410494002487127</v>
       </c>
       <c r="AH2" t="n">
-        <v>12298.1037412388</v>
+        <v>0.00306499063281215</v>
       </c>
       <c r="AI2" t="n">
-        <v>17035.2957723486</v>
+        <v>0.0122816404739317</v>
       </c>
       <c r="AJ2" t="n">
-        <v>12768.3624933617</v>
+        <v>0.00304841892547369</v>
       </c>
       <c r="AK2" t="n">
-        <v>9912.675200476</v>
+        <v>0.000654666414933222</v>
       </c>
       <c r="AL2" t="n">
-        <v>15654.9052113797</v>
+        <v>0.00628293228499559</v>
       </c>
       <c r="AM2" t="n">
-        <v>9562.63284260006</v>
+        <v>0.000444405181865187</v>
       </c>
       <c r="AN2" t="n">
-        <v>10063.3100325856</v>
+        <v>0.000659965957749407</v>
       </c>
       <c r="AO2" t="n">
-        <v>6979.60010879075</v>
+        <v>0.00110500222193367</v>
       </c>
       <c r="AP2" t="n">
-        <v>-1817.9575465715</v>
+        <v>0</v>
       </c>
       <c r="AQ2" t="n">
-        <v>-30923.0320993982</v>
+        <v>-0.0169600810425889</v>
       </c>
       <c r="AR2" t="n">
-        <v>-18678.9261874474</v>
+        <v>-0.0119444840139767</v>
       </c>
       <c r="AS2" t="n">
-        <v>9819.42166881295</v>
+        <v>0.00125396849546878</v>
       </c>
       <c r="AT2" t="n">
-        <v>-4877.81233719491</v>
+        <v>-0.00627330640791115</v>
       </c>
       <c r="AU2" t="n">
-        <v>10678.1595436077</v>
+        <v>0.00086513660730614</v>
       </c>
       <c r="AV2" t="n">
-        <v>-5209.3241717191</v>
+        <v>0</v>
       </c>
       <c r="AW2" t="n">
-        <v>7170.3861469535</v>
+        <v>0.000689210528692942</v>
       </c>
       <c r="AX2" t="n">
-        <v>-7541.80320048896</v>
+        <v>0</v>
       </c>
       <c r="AY2" t="n">
-        <v>17016.08884572</v>
+        <v>0.0177292571183268</v>
       </c>
       <c r="AZ2" t="n">
-        <v>-191.731510324487</v>
+        <v>-0.000774423179377822</v>
       </c>
       <c r="BA2" t="n">
-        <v>-58701.4782702935</v>
+        <v>-0.0306953923805776</v>
       </c>
       <c r="BB2" t="n">
-        <v>16901.2204384</v>
+        <v>0.0155587981274566</v>
       </c>
       <c r="BC2" t="n">
-        <v>-11237.4106685738</v>
+        <v>-0.00925562788127847</v>
       </c>
       <c r="BD2" t="n">
-        <v>13756.3198902172</v>
+        <v>0.00251791918166959</v>
       </c>
       <c r="BE2" t="n">
-        <v>-2257.9968830612</v>
+        <v>-0.00472857116732212</v>
       </c>
       <c r="BF2" t="n">
-        <v>1384.03067517952</v>
+        <v>0</v>
       </c>
       <c r="BG2" t="n">
-        <v>-5367.61270107695</v>
+        <v>-0.00643959705411009</v>
       </c>
       <c r="BH2" t="n">
-        <v>2725.25946106459</v>
+        <v>0</v>
       </c>
       <c r="BI2" t="n">
-        <v>13580.1051116818</v>
+        <v>0.00283614798395324</v>
       </c>
       <c r="BJ2" t="n">
-        <v>11486.0096102511</v>
+        <v>0.00163737134680268</v>
       </c>
       <c r="BK2" t="n">
-        <v>15651.9430212226</v>
+        <v>0.0110142177584514</v>
       </c>
       <c r="BL2" t="n">
-        <v>15791.6251236354</v>
+        <v>0.00965363467152715</v>
       </c>
       <c r="BM2" t="n">
-        <v>9048.83564421348</v>
+        <v>0.000508428649343776</v>
       </c>
       <c r="BN2" t="n">
-        <v>-6899.29000197058</v>
+        <v>-0.0000583683856867862</v>
       </c>
       <c r="BO2" t="n">
-        <v>11942.8427425644</v>
+        <v>0.00179682838237708</v>
       </c>
       <c r="BP2" t="n">
-        <v>4426.52415016258</v>
-      </c>
-      <c r="BQ2" t="n">
-        <v>12434.7328417095</v>
-      </c>
+        <v>0.000739703153161538</v>
+      </c>
+      <c r="BQ2"/>
       <c r="BR2" t="n">
-        <v>1073.29219409136</v>
+        <v>0.00359674469487541</v>
       </c>
       <c r="BS2" t="n">
-        <v>15646.4618111744</v>
+        <v>0</v>
       </c>
       <c r="BT2" t="n">
-        <v>-4668.73161350022</v>
+        <v>0.0114552119165973</v>
       </c>
       <c r="BU2" t="n">
-        <v>9327.51140504691</v>
+        <v>-0.00429388859354976</v>
       </c>
       <c r="BV2" t="n">
-        <v>10599.4100069251</v>
+        <v>0</v>
       </c>
       <c r="BW2" t="n">
-        <v>-12855.4988251964</v>
+        <v>0.000906494177921472</v>
       </c>
       <c r="BX2" t="n">
-        <v>-17125.8319192124</v>
+        <v>-0.00682513466869068</v>
       </c>
       <c r="BY2" t="n">
-        <v>-7134.3149813494</v>
+        <v>0</v>
       </c>
       <c r="BZ2" t="n">
-        <v>-27672.0544250038</v>
-      </c>
-      <c r="CA2" t="n">
-        <v>-5900.84416898472</v>
-      </c>
-      <c r="CB2" t="n">
-        <v>-2659.34931889673</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="CA2"/>
+      <c r="CB2"/>
       <c r="CC2" t="n">
-        <v>10529.4212553378</v>
+        <v>-0.00374143572943994</v>
       </c>
       <c r="CD2" t="n">
-        <v>-8651.97347527585</v>
+        <v>0.00194933285006078</v>
       </c>
       <c r="CE2" t="n">
-        <v>-9820.54455493437</v>
+        <v>0</v>
       </c>
       <c r="CF2" t="n">
-        <v>-36188.8754187354</v>
-      </c>
-      <c r="CG2" t="n">
-        <v>14817.2983279678</v>
-      </c>
+        <v>-0.00935283145433649</v>
+      </c>
+      <c r="CG2"/>
       <c r="CH2" t="n">
-        <v>4969.55626435118</v>
+        <v>0.00728525552765742</v>
       </c>
       <c r="CI2" t="n">
-        <v>15457.381627316</v>
+        <v>0</v>
       </c>
       <c r="CJ2" t="n">
-        <v>-7944.59008084716</v>
-      </c>
-      <c r="CK2" t="n">
-        <v>-102829.610291282</v>
-      </c>
-      <c r="CL2" t="n">
-        <v>16785.6092377773</v>
-      </c>
+        <v>0.00998666987943473</v>
+      </c>
+      <c r="CK2"/>
+      <c r="CL2"/>
       <c r="CM2" t="n">
-        <v>-3607.64170933012</v>
+        <v>0.00671133354183992</v>
       </c>
       <c r="CN2" t="n">
-        <v>13829.5948351565</v>
+        <v>0</v>
       </c>
       <c r="CO2" t="n">
-        <v>-18850.4742872436</v>
+        <v>0.00956506266535249</v>
       </c>
       <c r="CP2" t="n">
-        <v>13297.1564919992</v>
+        <v>0</v>
       </c>
       <c r="CQ2" t="n">
-        <v>4086.02200171107</v>
+        <v>0.00200525107845883</v>
       </c>
       <c r="CR2" t="n">
-        <v>-3804.88941329288</v>
+        <v>0.0000578468284673332</v>
       </c>
       <c r="CS2" t="n">
-        <v>-33097.2011246243</v>
+        <v>-0.00553938474617888</v>
       </c>
       <c r="CT2" t="n">
-        <v>-1508.93832848277</v>
+        <v>-0.0110407386582607</v>
       </c>
       <c r="CU2" t="n">
-        <v>-2100.20099147566</v>
+        <v>-0.00262095151439916</v>
       </c>
       <c r="CV2" t="n">
-        <v>-1498.48166087514</v>
+        <v>0</v>
       </c>
       <c r="CW2" t="n">
-        <v>16766.9960549584</v>
+        <v>0</v>
       </c>
       <c r="CX2" t="n">
-        <v>10511.6107185565</v>
+        <v>0.0139550253919775</v>
       </c>
       <c r="CY2" t="n">
-        <v>2133.47643948131</v>
+        <v>0.000504715696748122</v>
       </c>
       <c r="CZ2" t="n">
-        <v>-5749.04940860327</v>
+        <v>0.000420013155013044</v>
       </c>
       <c r="DA2" t="n">
-        <v>15477.7910928263</v>
+        <v>0</v>
       </c>
       <c r="DB2" t="n">
-        <v>-813.061536665345</v>
+        <v>0.00725845366622247</v>
       </c>
       <c r="DC2" t="n">
-        <v>17092.8765448279</v>
+        <v>-0.00476159627923135</v>
       </c>
       <c r="DD2" t="n">
-        <v>-1312.78556441275</v>
+        <v>0.00967838874412597</v>
       </c>
       <c r="DE2" t="n">
-        <v>-11533.1802764958</v>
-      </c>
-      <c r="DF2" t="n">
-        <v>13339.5551255168</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="DF2"/>
       <c r="DG2" t="n">
-        <v>10609.2015952821</v>
+        <v>0.00780054832898522</v>
       </c>
       <c r="DH2" t="n">
-        <v>-1640.25777131554</v>
-      </c>
-      <c r="DI2" t="n">
-        <v>17616.1150344981</v>
-      </c>
+        <v>0.00175218409449732</v>
+      </c>
+      <c r="DI2"/>
       <c r="DJ2" t="n">
-        <v>-30.3215656082084</v>
-      </c>
-      <c r="DK2" t="n">
-        <v>2852.73497761318</v>
-      </c>
+        <v>0.0243963930279728</v>
+      </c>
+      <c r="DK2"/>
       <c r="DL2" t="n">
-        <v>15778.1756675004</v>
+        <v>0</v>
       </c>
       <c r="DM2" t="n">
-        <v>12136.3301147471</v>
+        <v>0.0205940605211111</v>
       </c>
       <c r="DN2" t="n">
-        <v>11406.3018701038</v>
+        <v>0.00182679848860471</v>
       </c>
       <c r="DO2" t="n">
-        <v>-19879.7115834289</v>
+        <v>0.00149061479157976</v>
       </c>
       <c r="DP2" t="n">
-        <v>-10289.9238959513</v>
+        <v>-0.0118806388077742</v>
       </c>
       <c r="DQ2" t="n">
-        <v>16985.2702056833</v>
+        <v>-0.00815345515943452</v>
       </c>
       <c r="DR2" t="n">
-        <v>-8590.62523413244</v>
+        <v>0.0141778587263339</v>
       </c>
       <c r="DS2" t="n">
-        <v>-37579.0988769607</v>
-      </c>
-      <c r="DT2" t="n">
-        <v>14338.194923551</v>
-      </c>
+        <v>-0.00825860748085086</v>
+      </c>
+      <c r="DT2"/>
       <c r="DU2" t="n">
-        <v>2357.10246309846</v>
+        <v>0.00573605320307047</v>
       </c>
       <c r="DV2" t="n">
-        <v>5511.63228623028</v>
+        <v>-0.00433530877879111</v>
       </c>
       <c r="DW2" t="n">
-        <v>14896.8902505888</v>
+        <v>0.00047698724543377</v>
       </c>
       <c r="DX2" t="n">
-        <v>15166.2068776126</v>
+        <v>0.00445430222296178</v>
       </c>
       <c r="DY2" t="n">
-        <v>-14895.5998137553</v>
+        <v>0.00653278217144444</v>
       </c>
       <c r="DZ2" t="n">
-        <v>-2432.34911529656</v>
+        <v>-0.00965151222961706</v>
       </c>
       <c r="EA2" t="n">
-        <v>10493.7663074262</v>
+        <v>-0.000193952609045612</v>
       </c>
       <c r="EB2" t="n">
-        <v>-166794.162609226</v>
-      </c>
-      <c r="EC2" t="n">
-        <v>-2388.64348207187</v>
-      </c>
+        <v>0.000902342706480571</v>
+      </c>
+      <c r="EC2"/>
       <c r="ED2" t="n">
-        <v>-17137.7337287755</v>
-      </c>
-      <c r="EE2" t="n">
-        <v>17631.6392490078</v>
-      </c>
+        <v>-0.00323388169270435</v>
+      </c>
+      <c r="EE2"/>
       <c r="EF2" t="n">
-        <v>-69432.4445458381</v>
-      </c>
-      <c r="EG2" t="n">
-        <v>12066.9303245658</v>
-      </c>
+        <v>0.0160640774466487</v>
+      </c>
+      <c r="EG2"/>
       <c r="EH2" t="n">
-        <v>11862.8284232503</v>
+        <v>0.00332306840230412</v>
       </c>
       <c r="EI2" t="n">
-        <v>-6703.16990442176</v>
-      </c>
-      <c r="EJ2" t="n">
-        <v>17048.5571990399</v>
-      </c>
+        <v>0.00268837678385215</v>
+      </c>
+      <c r="EJ2"/>
       <c r="EK2" t="n">
-        <v>16420.1874072007</v>
+        <v>0.0179558707837201</v>
       </c>
       <c r="EL2" t="n">
-        <v>12466.4044135369</v>
+        <v>0.0159718112421604</v>
       </c>
       <c r="EM2" t="n">
-        <v>17455.6458351046</v>
+        <v>0.00325966061619425</v>
       </c>
       <c r="EN2" t="n">
-        <v>-4652.94079303275</v>
+        <v>0.00747564608430084</v>
       </c>
       <c r="EO2" t="n">
-        <v>15171.7331727909</v>
+        <v>0</v>
       </c>
       <c r="EP2" t="n">
-        <v>-1525.01735014429</v>
+        <v>0.0139052291085141</v>
       </c>
       <c r="EQ2" t="n">
-        <v>-11588.3270755132</v>
+        <v>0.000356401444898818</v>
       </c>
       <c r="ER2" t="n">
-        <v>-6912.78346043721</v>
+        <v>-0.00986778490493046</v>
       </c>
       <c r="ES2" t="n">
-        <v>110.133953433044</v>
+        <v>-0.00496364984952597</v>
       </c>
       <c r="ET2" t="n">
-        <v>10603.012643428</v>
+        <v>-0.00418096634146452</v>
       </c>
       <c r="EU2" t="n">
-        <v>-6517.51437804776</v>
+        <v>0.000742046527091167</v>
       </c>
       <c r="EV2" t="n">
-        <v>17740.6049969009</v>
+        <v>0</v>
       </c>
       <c r="EW2" t="n">
-        <v>12855.797795435</v>
+        <v>0.018447524133669</v>
       </c>
       <c r="EX2" t="n">
-        <v>3039.44864041607</v>
-      </c>
-      <c r="EY2" t="n">
-        <v>15311.2561301849</v>
-      </c>
+        <v>0.00641068097009834</v>
+      </c>
+      <c r="EY2"/>
       <c r="EZ2" t="n">
-        <v>-56132.1319076443</v>
-      </c>
-      <c r="FA2" t="n">
-        <v>16192.4798364847</v>
-      </c>
+        <v>0.00694460606538522</v>
+      </c>
+      <c r="FA2"/>
       <c r="FB2" t="n">
-        <v>-124640.136145221</v>
-      </c>
-      <c r="FC2" t="n">
-        <v>-3578.15095876736</v>
-      </c>
+        <v>0.0033207298063737</v>
+      </c>
+      <c r="FC2"/>
       <c r="FD2" t="n">
-        <v>-7832.52087162107</v>
-      </c>
-      <c r="FE2" t="n">
-        <v>-6920.08857310577</v>
-      </c>
-      <c r="FF2" t="n">
-        <v>15629.7651180677</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="FE2"/>
+      <c r="FF2"/>
       <c r="FG2" t="n">
-        <v>16836.4140139931</v>
+        <v>0.00823372919088676</v>
       </c>
       <c r="FH2" t="n">
-        <v>-7452.73469595688</v>
+        <v>0.0126736614267342</v>
       </c>
       <c r="FI2" t="n">
-        <v>5127.54097694829</v>
+        <v>0</v>
       </c>
       <c r="FJ2" t="n">
-        <v>-44981.1104488244</v>
-      </c>
-      <c r="FK2" t="n">
-        <v>-3972.5876437022</v>
-      </c>
+        <v>-0.000943463651716223</v>
+      </c>
+      <c r="FK2"/>
       <c r="FL2" t="n">
-        <v>6313.56168273922</v>
+        <v>0</v>
       </c>
       <c r="FM2" t="n">
-        <v>5270.31377883656</v>
+        <v>0.000986391210062495</v>
       </c>
       <c r="FN2" t="n">
-        <v>16237.0260180271</v>
+        <v>0</v>
       </c>
       <c r="FO2" t="n">
-        <v>14575.6450582973</v>
+        <v>0.0126098883587276</v>
       </c>
       <c r="FP2" t="n">
-        <v>7194.88355404671</v>
+        <v>0.00521601773520042</v>
       </c>
       <c r="FQ2" t="n">
-        <v>-18601.19458814</v>
+        <v>0.00111634929055457</v>
       </c>
       <c r="FR2" t="n">
-        <v>14840.5533892637</v>
+        <v>0</v>
       </c>
       <c r="FS2" t="n">
-        <v>1869.13853971949</v>
+        <v>0.00420498272175106</v>
       </c>
       <c r="FT2" t="n">
-        <v>9368.80966140435</v>
+        <v>0.000218148523181066</v>
+      </c>
+      <c r="FU2" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GCP max_gain, prudent map update
</commit_message>
<xml_diff>
--- a/xlsx/'folder' missing.xlsx
+++ b/xlsx/'folder' missing.xlsx
@@ -545,7 +545,7 @@
     <t xml:space="preserve">North Korea</t>
   </si>
   <si>
-    <t xml:space="preserve">Scentral_npv_over_gdp_gcs_adj</t>
+    <t xml:space="preserve">Sprudent_npv_over_gdp_gcs_adj</t>
   </si>
 </sst>
 </file>
@@ -1415,49 +1415,49 @@
         <v>177</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0181978479454534</v>
+        <v>0.0151043838170846</v>
       </c>
       <c r="C2" t="n">
-        <v>0.00605031278738703</v>
+        <v>0.00359379866853409</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2"/>
       <c r="F2" t="n">
-        <v>0.000478969338267119</v>
+        <v>0.000410639911282762</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2"/>
       <c r="I2" t="n">
-        <v>-0.00865528391275657</v>
+        <v>-0.00906753310710586</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0.023278051478139</v>
+        <v>0.0197357646957889</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.0106350667875789</v>
+        <v>-0.0110574671035766</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0046695949530543</v>
+        <v>0.00281927431191736</v>
       </c>
       <c r="N2" t="n">
-        <v>0.0150994491515351</v>
+        <v>0.0123989249979428</v>
       </c>
       <c r="O2" t="n">
-        <v>0.00885096520762095</v>
+        <v>0.0070820295521727</v>
       </c>
       <c r="P2" t="n">
-        <v>-0.0045165510205679</v>
+        <v>-0.00465620993605702</v>
       </c>
       <c r="Q2"/>
       <c r="R2" t="n">
-        <v>0.000359472231601866</v>
+        <v>0.000289105637803429</v>
       </c>
       <c r="S2" t="n">
         <v>0</v>
@@ -1466,16 +1466,16 @@
         <v>0</v>
       </c>
       <c r="U2" t="n">
-        <v>0.0013842547654194</v>
+        <v>0.000876068697373236</v>
       </c>
       <c r="V2" t="n">
-        <v>0.000741413449639804</v>
+        <v>0.000623788839979223</v>
       </c>
       <c r="W2" t="n">
-        <v>0.000608722598182665</v>
+        <v>0.000514636877426194</v>
       </c>
       <c r="X2" t="n">
-        <v>0.000971757976059452</v>
+        <v>0.000805313115135587</v>
       </c>
       <c r="Y2"/>
       <c r="Z2" t="n">
@@ -1485,145 +1485,141 @@
         <v>0</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.0329172745649323</v>
+        <v>0.0273964563325208</v>
       </c>
       <c r="AC2"/>
-      <c r="AD2" t="n">
-        <v>-0.00349480425447978</v>
-      </c>
+      <c r="AD2"/>
       <c r="AE2"/>
       <c r="AF2" t="n">
         <v>0</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.000410494002487127</v>
+        <v>0.000156350839541344</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.00306499063281215</v>
+        <v>0.00181616904949319</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.0122816404739317</v>
+        <v>0.0102379030134157</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.00304841892547369</v>
+        <v>0.00170710968242554</v>
       </c>
       <c r="AK2" t="n">
-        <v>0.000654666414933222</v>
+        <v>0.000512474295276406</v>
       </c>
       <c r="AL2" t="n">
-        <v>0.00628293228499559</v>
+        <v>0.00496401053353295</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.000444405181865187</v>
+        <v>0.00004134735942103</v>
       </c>
       <c r="AN2" t="n">
-        <v>0.000659965957749407</v>
+        <v>0.00046950652686288</v>
       </c>
       <c r="AO2" t="n">
-        <v>0.00110500222193367</v>
+        <v>0.000911133887080572</v>
       </c>
       <c r="AP2" t="n">
         <v>0</v>
       </c>
       <c r="AQ2" t="n">
-        <v>-0.0169600810425889</v>
+        <v>-0.017371844776287</v>
       </c>
       <c r="AR2" t="n">
-        <v>-0.0119444840139767</v>
+        <v>-0.0123825197143604</v>
       </c>
       <c r="AS2" t="n">
-        <v>0.00125396849546878</v>
+        <v>0.000574858850398968</v>
       </c>
       <c r="AT2" t="n">
-        <v>-0.00627330640791115</v>
+        <v>-0.00671104301656217</v>
       </c>
       <c r="AU2" t="n">
-        <v>0.00086513660730614</v>
+        <v>0.000511633593603243</v>
       </c>
       <c r="AV2" t="n">
         <v>0</v>
       </c>
       <c r="AW2" t="n">
-        <v>0.000689210528692942</v>
+        <v>0.000580556903979908</v>
       </c>
       <c r="AX2" t="n">
         <v>0</v>
       </c>
       <c r="AY2" t="n">
-        <v>0.0177292571183268</v>
+        <v>0.014770077126678</v>
       </c>
       <c r="AZ2" t="n">
-        <v>-0.000774423179377822</v>
+        <v>-0.000880917648465152</v>
       </c>
       <c r="BA2" t="n">
-        <v>-0.0306953923805776</v>
+        <v>-0.0311435299324767</v>
       </c>
       <c r="BB2" t="n">
-        <v>0.0155587981274566</v>
+        <v>0.0129126162029414</v>
       </c>
       <c r="BC2" t="n">
-        <v>-0.00925562788127847</v>
+        <v>-0.00970686304218662</v>
       </c>
       <c r="BD2" t="n">
-        <v>0.00251791918166959</v>
+        <v>0.00151572673886781</v>
       </c>
       <c r="BE2" t="n">
-        <v>-0.00472857116732212</v>
+        <v>-0.00515433738859531</v>
       </c>
       <c r="BF2" t="n">
         <v>0</v>
       </c>
-      <c r="BG2" t="n">
-        <v>-0.00643959705411009</v>
-      </c>
+      <c r="BG2"/>
       <c r="BH2" t="n">
         <v>0</v>
       </c>
       <c r="BI2" t="n">
-        <v>0.00283614798395324</v>
+        <v>0.00191845711714543</v>
       </c>
       <c r="BJ2" t="n">
-        <v>0.00163737134680268</v>
+        <v>0.00101119869884897</v>
       </c>
       <c r="BK2" t="n">
-        <v>0.0110142177584514</v>
+        <v>0.00867115959277107</v>
       </c>
       <c r="BL2" t="n">
-        <v>0.00965363467152715</v>
+        <v>0.00768467925022399</v>
       </c>
       <c r="BM2" t="n">
-        <v>0.000508428649343776</v>
+        <v>0.000435977988835038</v>
       </c>
       <c r="BN2" t="n">
-        <v>-0.0000583683856867862</v>
+        <v>-0.000062918905487202</v>
       </c>
       <c r="BO2" t="n">
-        <v>0.00179682838237708</v>
+        <v>0.000997688315160532</v>
       </c>
       <c r="BP2" t="n">
-        <v>0.000739703153161538</v>
+        <v>0.000627857482623868</v>
       </c>
       <c r="BQ2"/>
       <c r="BR2" t="n">
-        <v>0.00359674469487541</v>
+        <v>0.00193630465305304</v>
       </c>
       <c r="BS2" t="n">
         <v>0</v>
       </c>
       <c r="BT2" t="n">
-        <v>0.0114552119165973</v>
+        <v>0.00911271981117367</v>
       </c>
       <c r="BU2" t="n">
-        <v>-0.00429388859354976</v>
+        <v>-0.0045623288140523</v>
       </c>
       <c r="BV2" t="n">
         <v>0</v>
       </c>
       <c r="BW2" t="n">
-        <v>0.000906494177921472</v>
+        <v>0.0000481930823676458</v>
       </c>
       <c r="BX2" t="n">
-        <v>-0.00682513466869068</v>
+        <v>-0.00713749142471962</v>
       </c>
       <c r="BY2" t="n">
         <v>0</v>
@@ -1634,55 +1630,53 @@
       <c r="CA2"/>
       <c r="CB2"/>
       <c r="CC2" t="n">
-        <v>-0.00374143572943994</v>
+        <v>-0.00407972585902377</v>
       </c>
       <c r="CD2" t="n">
-        <v>0.00194933285006078</v>
+        <v>0.00145364858923396</v>
       </c>
       <c r="CE2" t="n">
         <v>0</v>
       </c>
-      <c r="CF2" t="n">
-        <v>-0.00935283145433649</v>
-      </c>
+      <c r="CF2"/>
       <c r="CG2"/>
       <c r="CH2" t="n">
-        <v>0.00728525552765742</v>
+        <v>0.00547561253493542</v>
       </c>
       <c r="CI2" t="n">
         <v>0</v>
       </c>
       <c r="CJ2" t="n">
-        <v>0.00998666987943473</v>
+        <v>0.00810508653352903</v>
       </c>
       <c r="CK2"/>
       <c r="CL2"/>
       <c r="CM2" t="n">
-        <v>0.00671133354183992</v>
+        <v>0.00563660850327913</v>
       </c>
       <c r="CN2" t="n">
         <v>0</v>
       </c>
       <c r="CO2" t="n">
-        <v>0.00956506266535249</v>
+        <v>0.00688455444802085</v>
       </c>
       <c r="CP2" t="n">
         <v>0</v>
       </c>
       <c r="CQ2" t="n">
-        <v>0.00200525107845883</v>
+        <v>0.00031973800393597</v>
       </c>
       <c r="CR2" t="n">
-        <v>0.0000578468284673332</v>
+        <v>0</v>
       </c>
       <c r="CS2" t="n">
-        <v>-0.00553938474617888</v>
+        <v>-0.00594978512968433</v>
       </c>
       <c r="CT2" t="n">
-        <v>-0.0110407386582607</v>
+        <v>-0.0113123376260774</v>
       </c>
       <c r="CU2" t="n">
-        <v>-0.00262095151439916</v>
+        <v>-0.00285742455829926</v>
       </c>
       <c r="CV2" t="n">
         <v>0</v>
@@ -1691,155 +1685,151 @@
         <v>0</v>
       </c>
       <c r="CX2" t="n">
-        <v>0.0139550253919775</v>
+        <v>0.0115300983234055</v>
       </c>
       <c r="CY2" t="n">
-        <v>0.000504715696748122</v>
+        <v>0</v>
       </c>
       <c r="CZ2" t="n">
-        <v>0.000420013155013044</v>
+        <v>0.000358727919134943</v>
       </c>
       <c r="DA2" t="n">
         <v>0</v>
       </c>
       <c r="DB2" t="n">
-        <v>0.00725845366622247</v>
+        <v>0.0056792195898242</v>
       </c>
       <c r="DC2" t="n">
-        <v>-0.00476159627923135</v>
+        <v>-0.00521040600490127</v>
       </c>
       <c r="DD2" t="n">
-        <v>0.00967838874412597</v>
+        <v>0.00804082587520934</v>
       </c>
       <c r="DE2" t="n">
         <v>0</v>
       </c>
       <c r="DF2"/>
       <c r="DG2" t="n">
-        <v>0.00780054832898522</v>
+        <v>0.00531935055390146</v>
       </c>
       <c r="DH2" t="n">
-        <v>0.00175218409449732</v>
+        <v>0.000722589352761333</v>
       </c>
       <c r="DI2"/>
       <c r="DJ2" t="n">
-        <v>0.0243963930279728</v>
+        <v>0.0206837377157536</v>
       </c>
       <c r="DK2"/>
       <c r="DL2" t="n">
         <v>0</v>
       </c>
       <c r="DM2" t="n">
-        <v>0.0205940605211111</v>
+        <v>0.0163720718627636</v>
       </c>
       <c r="DN2" t="n">
-        <v>0.00182679848860471</v>
+        <v>0.000995848385274252</v>
       </c>
       <c r="DO2" t="n">
-        <v>0.00149061479157976</v>
+        <v>0.000931642352597824</v>
       </c>
       <c r="DP2" t="n">
-        <v>-0.0118806388077742</v>
-      </c>
-      <c r="DQ2" t="n">
-        <v>-0.00815345515943452</v>
-      </c>
+        <v>-0.0122990023591668</v>
+      </c>
+      <c r="DQ2"/>
       <c r="DR2" t="n">
-        <v>0.0141778587263339</v>
-      </c>
-      <c r="DS2" t="n">
-        <v>-0.00825860748085086</v>
-      </c>
+        <v>0.0118578424122401</v>
+      </c>
+      <c r="DS2"/>
       <c r="DT2"/>
       <c r="DU2" t="n">
-        <v>0.00573605320307047</v>
+        <v>0.00423373735789115</v>
       </c>
       <c r="DV2" t="n">
-        <v>-0.00433530877879111</v>
+        <v>-0.00205414744280956</v>
       </c>
       <c r="DW2" t="n">
-        <v>0.00047698724543377</v>
+        <v>0.000408714782782181</v>
       </c>
       <c r="DX2" t="n">
-        <v>0.00445430222296178</v>
+        <v>0.00321012755637867</v>
       </c>
       <c r="DY2" t="n">
-        <v>0.00653278217144444</v>
+        <v>0.00485096659966935</v>
       </c>
       <c r="DZ2" t="n">
-        <v>-0.00965151222961706</v>
+        <v>-0.00997287707281265</v>
       </c>
       <c r="EA2" t="n">
-        <v>-0.000193952609045612</v>
+        <v>-0.000218165248823758</v>
       </c>
       <c r="EB2" t="n">
-        <v>0.000902342706480571</v>
+        <v>0.000551340277322914</v>
       </c>
       <c r="EC2"/>
       <c r="ED2" t="n">
-        <v>-0.00323388169270435</v>
+        <v>-0.00347339128967313</v>
       </c>
       <c r="EE2"/>
       <c r="EF2" t="n">
-        <v>0.0160640774466487</v>
+        <v>0.0136249242800312</v>
       </c>
       <c r="EG2"/>
       <c r="EH2" t="n">
-        <v>0.00332306840230412</v>
+        <v>0.0022793872973777</v>
       </c>
       <c r="EI2" t="n">
-        <v>0.00268837678385215</v>
+        <v>0.00158428263815852</v>
       </c>
       <c r="EJ2"/>
       <c r="EK2" t="n">
-        <v>0.0179558707837201</v>
+        <v>0.0148941046820604</v>
       </c>
       <c r="EL2" t="n">
-        <v>0.0159718112421604</v>
+        <v>0.0130299989590248</v>
       </c>
       <c r="EM2" t="n">
-        <v>0.00325966061619425</v>
+        <v>0.001714630929229</v>
       </c>
       <c r="EN2" t="n">
-        <v>0.00747564608430084</v>
+        <v>0.00631057285234826</v>
       </c>
       <c r="EO2" t="n">
         <v>0</v>
       </c>
       <c r="EP2" t="n">
-        <v>0.0139052291085141</v>
+        <v>0.0112928448214244</v>
       </c>
       <c r="EQ2" t="n">
-        <v>0.000356401444898818</v>
+        <v>0.000306592455004204</v>
       </c>
       <c r="ER2" t="n">
-        <v>-0.00986778490493046</v>
+        <v>-0.0103121841994999</v>
       </c>
       <c r="ES2" t="n">
-        <v>-0.00496364984952597</v>
+        <v>-0.00523376878821256</v>
       </c>
       <c r="ET2" t="n">
-        <v>-0.00418096634146452</v>
+        <v>-0.00461662233276537</v>
       </c>
       <c r="EU2" t="n">
-        <v>0.000742046527091167</v>
+        <v>0.000289396351640338</v>
       </c>
       <c r="EV2" t="n">
         <v>0</v>
       </c>
       <c r="EW2" t="n">
-        <v>0.018447524133669</v>
+        <v>0.0156906420238651</v>
       </c>
       <c r="EX2" t="n">
-        <v>0.00641068097009834</v>
+        <v>0.00427737927459854</v>
       </c>
       <c r="EY2"/>
       <c r="EZ2" t="n">
-        <v>0.00694460606538522</v>
+        <v>0.00543701416122187</v>
       </c>
       <c r="FA2"/>
       <c r="FB2" t="n">
-        <v>0</v>
+        <v>0.00244177260296653</v>
       </c>
       <c r="FC2"/>
       <c r="FD2" t="n">
@@ -1848,44 +1838,44 @@
       <c r="FE2"/>
       <c r="FF2"/>
       <c r="FG2" t="n">
-        <v>0.00823372919088676</v>
+        <v>0.0064762855540297</v>
       </c>
       <c r="FH2" t="n">
-        <v>0.0126736614267342</v>
+        <v>0.0104949467258887</v>
       </c>
       <c r="FI2" t="n">
         <v>0</v>
       </c>
       <c r="FJ2" t="n">
-        <v>-0.000943463651716223</v>
+        <v>-0.000536334110083664</v>
       </c>
       <c r="FK2"/>
       <c r="FL2" t="n">
         <v>0</v>
       </c>
       <c r="FM2" t="n">
-        <v>0.000986391210062495</v>
+        <v>0.000831871945226889</v>
       </c>
       <c r="FN2" t="n">
         <v>0</v>
       </c>
       <c r="FO2" t="n">
-        <v>0.0126098883587276</v>
+        <v>0.0100872572897246</v>
       </c>
       <c r="FP2" t="n">
-        <v>0.00521601773520042</v>
+        <v>0.00360472029934705</v>
       </c>
       <c r="FQ2" t="n">
-        <v>0.00111634929055457</v>
+        <v>0.000112782239843026</v>
       </c>
       <c r="FR2" t="n">
         <v>0</v>
       </c>
       <c r="FS2" t="n">
-        <v>0.00420498272175106</v>
+        <v>0.00318834924369617</v>
       </c>
       <c r="FT2" t="n">
-        <v>0.000218148523181066</v>
+        <v>0.0000349231624274589</v>
       </c>
       <c r="FU2" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
map of combined tax
</commit_message>
<xml_diff>
--- a/xlsx/'folder' missing.xlsx
+++ b/xlsx/'folder' missing.xlsx
@@ -404,6 +404,9 @@
     <t xml:space="preserve">Poland</t>
   </si>
   <si>
+    <t xml:space="preserve">North Korea</t>
+  </si>
+  <si>
     <t xml:space="preserve">Portugal</t>
   </si>
   <si>
@@ -542,10 +545,7 @@
     <t xml:space="preserve">Zimbabwe</t>
   </si>
   <si>
-    <t xml:space="preserve">North Korea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprudent_npv_over_gdp_gcs_adj</t>
+    <t xml:space="preserve">net_gain_all_taxes_pc</t>
   </si>
 </sst>
 </file>
@@ -1414,471 +1414,515 @@
       <c r="A2" t="s">
         <v>177</v>
       </c>
-      <c r="B2" t="n">
-        <v>0.0151043838170846</v>
-      </c>
+      <c r="B2"/>
       <c r="C2" t="n">
-        <v>0.00359379866853409</v>
+        <v>143.409393886515</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2"/>
+        <v>168.639558819865</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-1100.97513405339</v>
+      </c>
       <c r="F2" t="n">
-        <v>0.000410639911282762</v>
+        <v>6.25570550147051</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2"/>
+        <v>152.758299538036</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-1289.9146083007</v>
+      </c>
       <c r="I2" t="n">
-        <v>-0.00906753310710586</v>
+        <v>-547.053671471371</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>146.951557918648</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0197357646957889</v>
+        <v>207.088311245121</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.0110574671035766</v>
+        <v>-275.176706448841</v>
       </c>
       <c r="M2" t="n">
-        <v>0.00281927431191736</v>
+        <v>204.229050977001</v>
       </c>
       <c r="N2" t="n">
-        <v>0.0123989249979428</v>
+        <v>206.46864253029</v>
       </c>
       <c r="O2" t="n">
-        <v>0.0070820295521727</v>
+        <v>260.859226667799</v>
       </c>
       <c r="P2" t="n">
-        <v>-0.00465620993605702</v>
-      </c>
-      <c r="Q2"/>
+        <v>-7.98184572698369</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>-431.792746475264</v>
+      </c>
       <c r="R2" t="n">
-        <v>0.000289105637803429</v>
+        <v>-273.303735512854</v>
       </c>
       <c r="S2" t="n">
-        <v>0</v>
+        <v>167.996399987714</v>
       </c>
       <c r="T2" t="n">
-        <v>0</v>
+        <v>152.624378550863</v>
       </c>
       <c r="U2" t="n">
-        <v>0.000876068697373236</v>
+        <v>131.30627605769</v>
       </c>
       <c r="V2" t="n">
-        <v>0.000623788839979223</v>
+        <v>198.230011946533</v>
       </c>
       <c r="W2" t="n">
-        <v>0.000514636877426194</v>
+        <v>59.4445327500726</v>
       </c>
       <c r="X2" t="n">
-        <v>0.000805313115135587</v>
-      </c>
-      <c r="Y2"/>
-      <c r="Z2" t="n">
-        <v>0</v>
-      </c>
+        <v>-106.492298242389</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>-371.587532192645</v>
+      </c>
+      <c r="Z2"/>
       <c r="AA2" t="n">
-        <v>0</v>
+        <v>134.324446810054</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.0273964563325208</v>
-      </c>
-      <c r="AC2"/>
-      <c r="AD2"/>
-      <c r="AE2"/>
+        <v>195.859887451739</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>-558.549211353626</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>-1800.62183091095</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>-84.0049854705434</v>
+      </c>
       <c r="AF2" t="n">
-        <v>0</v>
+        <v>-10.6778367752665</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.000156350839541344</v>
+        <v>183.133990704133</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.00181616904949319</v>
+        <v>195.660364897698</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.0102379030134157</v>
+        <v>206.930361809342</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.00170710968242554</v>
+        <v>126.086429908275</v>
       </c>
       <c r="AK2" t="n">
-        <v>0.000512474295276406</v>
+        <v>140.308494736565</v>
       </c>
       <c r="AL2" t="n">
-        <v>0.00496401053353295</v>
+        <v>215.31818437111</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.00004134735942103</v>
+        <v>212.088613947147</v>
       </c>
       <c r="AN2" t="n">
-        <v>0.00046950652686288</v>
-      </c>
-      <c r="AO2" t="n">
-        <v>0.000911133887080572</v>
-      </c>
+        <v>-39.9837424779363</v>
+      </c>
+      <c r="AO2"/>
       <c r="AP2" t="n">
-        <v>0</v>
+        <v>-244.882731674327</v>
       </c>
       <c r="AQ2" t="n">
-        <v>-0.017371844776287</v>
+        <v>-232.920617912088</v>
       </c>
       <c r="AR2" t="n">
-        <v>-0.0123825197143604</v>
+        <v>-511.438215541767</v>
       </c>
       <c r="AS2" t="n">
-        <v>0.000574858850398968</v>
+        <v>213.654391234779</v>
       </c>
       <c r="AT2" t="n">
-        <v>-0.00671104301656217</v>
+        <v>-1235.38854581829</v>
       </c>
       <c r="AU2" t="n">
-        <v>0.000511633593603243</v>
+        <v>93.5675998633401</v>
       </c>
       <c r="AV2" t="n">
-        <v>0</v>
+        <v>170.077713417708</v>
       </c>
       <c r="AW2" t="n">
-        <v>0.000580556903979908</v>
+        <v>155.51960535635</v>
       </c>
       <c r="AX2" t="n">
-        <v>0</v>
+        <v>196.092803195308</v>
       </c>
       <c r="AY2" t="n">
-        <v>0.014770077126678</v>
+        <v>224.471045387976</v>
       </c>
       <c r="AZ2" t="n">
-        <v>-0.000880917648465152</v>
+        <v>-230.246152472394</v>
       </c>
       <c r="BA2" t="n">
-        <v>-0.0311435299324767</v>
+        <v>-249.544431020225</v>
       </c>
       <c r="BB2" t="n">
-        <v>0.0129126162029414</v>
+        <v>218.766745173625</v>
       </c>
       <c r="BC2" t="n">
-        <v>-0.00970686304218662</v>
+        <v>-397.311912018252</v>
       </c>
       <c r="BD2" t="n">
-        <v>0.00151572673886781</v>
+        <v>39.5341913664369</v>
       </c>
       <c r="BE2" t="n">
-        <v>-0.00515433738859531</v>
+        <v>-610.361066380005</v>
       </c>
       <c r="BF2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG2"/>
+        <v>-4.0258132605518</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>-1385.00415909099</v>
+      </c>
       <c r="BH2" t="n">
-        <v>0</v>
+        <v>134.076255786894</v>
       </c>
       <c r="BI2" t="n">
-        <v>0.00191845711714543</v>
+        <v>200.678897196908</v>
       </c>
       <c r="BJ2" t="n">
-        <v>0.00101119869884897</v>
+        <v>150.097292493941</v>
       </c>
       <c r="BK2" t="n">
-        <v>0.00867115959277107</v>
+        <v>207.817210836551</v>
       </c>
       <c r="BL2" t="n">
-        <v>0.00768467925022399</v>
+        <v>217.456104803615</v>
       </c>
       <c r="BM2" t="n">
-        <v>0.000435977988835038</v>
+        <v>-45.8573113096867</v>
       </c>
       <c r="BN2" t="n">
-        <v>-0.000062918905487202</v>
+        <v>-229.797584749281</v>
       </c>
       <c r="BO2" t="n">
-        <v>0.000997688315160532</v>
+        <v>165.482294745936</v>
       </c>
       <c r="BP2" t="n">
-        <v>0.000627857482623868</v>
+        <v>-94.5863298432474</v>
       </c>
       <c r="BQ2"/>
       <c r="BR2" t="n">
-        <v>0.00193630465305304</v>
+        <v>217.511718475224</v>
       </c>
       <c r="BS2" t="n">
-        <v>0</v>
+        <v>-127.169910133841</v>
       </c>
       <c r="BT2" t="n">
-        <v>0.00911271981117367</v>
+        <v>238.433435388084</v>
       </c>
       <c r="BU2" t="n">
-        <v>-0.0045623288140523</v>
+        <v>-55.6106095555704</v>
       </c>
       <c r="BV2" t="n">
-        <v>0</v>
+        <v>195.45238156266</v>
       </c>
       <c r="BW2" t="n">
-        <v>0.0000481930823676458</v>
+        <v>224.407637557826</v>
       </c>
       <c r="BX2" t="n">
-        <v>-0.00713749142471962</v>
+        <v>-818.213639797646</v>
       </c>
       <c r="BY2" t="n">
-        <v>0</v>
+        <v>188.900694090682</v>
       </c>
       <c r="BZ2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CA2"/>
-      <c r="CB2"/>
+        <v>70.7718047161104</v>
+      </c>
+      <c r="CA2" t="n">
+        <v>-1861.18967704674</v>
+      </c>
+      <c r="CB2" t="n">
+        <v>-367.537086187999</v>
+      </c>
       <c r="CC2" t="n">
-        <v>-0.00407972585902377</v>
+        <v>-233.736263016668</v>
       </c>
       <c r="CD2" t="n">
-        <v>0.00145364858923396</v>
+        <v>160.841316743479</v>
       </c>
       <c r="CE2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CF2"/>
-      <c r="CG2"/>
+        <v>169.162837243482</v>
+      </c>
+      <c r="CF2" t="n">
+        <v>-264.635924166443</v>
+      </c>
+      <c r="CG2" t="n">
+        <v>2.43480496890075</v>
+      </c>
       <c r="CH2" t="n">
-        <v>0.00547561253493542</v>
+        <v>211.455307149995</v>
       </c>
       <c r="CI2" t="n">
-        <v>0</v>
+        <v>219.005838003631</v>
       </c>
       <c r="CJ2" t="n">
-        <v>0.00810508653352903</v>
-      </c>
-      <c r="CK2"/>
-      <c r="CL2"/>
+        <v>239.468724533638</v>
+      </c>
+      <c r="CK2" t="n">
+        <v>-224.201161289987</v>
+      </c>
+      <c r="CL2" t="n">
+        <v>-574.278596844366</v>
+      </c>
       <c r="CM2" t="n">
-        <v>0.00563660850327913</v>
+        <v>232.759302143842</v>
       </c>
       <c r="CN2" t="n">
-        <v>0</v>
+        <v>216.797485697664</v>
       </c>
       <c r="CO2" t="n">
-        <v>0.00688455444802085</v>
+        <v>211.985505455395</v>
       </c>
       <c r="CP2" t="n">
-        <v>0</v>
+        <v>105.150138933505</v>
       </c>
       <c r="CQ2" t="n">
-        <v>0.00031973800393597</v>
+        <v>214.091285005871</v>
       </c>
       <c r="CR2" t="n">
-        <v>0</v>
+        <v>241.321010947748</v>
       </c>
       <c r="CS2" t="n">
-        <v>-0.00594978512968433</v>
+        <v>-209.652183461914</v>
       </c>
       <c r="CT2" t="n">
-        <v>-0.0113123376260774</v>
+        <v>-3386.3416322839</v>
       </c>
       <c r="CU2" t="n">
-        <v>-0.00285742455829926</v>
+        <v>-217.361056427962</v>
       </c>
       <c r="CV2" t="n">
-        <v>0</v>
+        <v>204.356992684075</v>
       </c>
       <c r="CW2" t="n">
-        <v>0</v>
+        <v>186.462831948461</v>
       </c>
       <c r="CX2" t="n">
-        <v>0.0115300983234055</v>
+        <v>234.133175290046</v>
       </c>
       <c r="CY2" t="n">
-        <v>0</v>
+        <v>75.6966013677964</v>
       </c>
       <c r="CZ2" t="n">
-        <v>0.000358727919134943</v>
+        <v>24.5515982731845</v>
       </c>
       <c r="DA2" t="n">
-        <v>0</v>
+        <v>169.117449122951</v>
       </c>
       <c r="DB2" t="n">
-        <v>0.0056792195898242</v>
+        <v>192.698302979678</v>
       </c>
       <c r="DC2" t="n">
-        <v>-0.00521040600490127</v>
+        <v>-595.98411888471</v>
       </c>
       <c r="DD2" t="n">
-        <v>0.00804082587520934</v>
+        <v>268.803662829531</v>
       </c>
       <c r="DE2" t="n">
-        <v>0</v>
-      </c>
-      <c r="DF2"/>
+        <v>85.3270220511585</v>
+      </c>
+      <c r="DF2" t="n">
+        <v>165.435265264414</v>
+      </c>
       <c r="DG2" t="n">
-        <v>0.00531935055390146</v>
+        <v>203.525425910764</v>
       </c>
       <c r="DH2" t="n">
-        <v>0.000722589352761333</v>
-      </c>
-      <c r="DI2"/>
+        <v>132.901993880669</v>
+      </c>
+      <c r="DI2" t="n">
+        <v>-81.5724400104323</v>
+      </c>
       <c r="DJ2" t="n">
-        <v>0.0206837377157536</v>
-      </c>
-      <c r="DK2"/>
+        <v>213.734161298425</v>
+      </c>
+      <c r="DK2" t="n">
+        <v>-21.0091960911196</v>
+      </c>
       <c r="DL2" t="n">
-        <v>0</v>
+        <v>165.122118692209</v>
       </c>
       <c r="DM2" t="n">
-        <v>0.0163720718627636</v>
+        <v>193.164631427579</v>
       </c>
       <c r="DN2" t="n">
-        <v>0.000995848385274252</v>
+        <v>195.497146770179</v>
       </c>
       <c r="DO2" t="n">
-        <v>0.000931642352597824</v>
+        <v>228.213887238075</v>
       </c>
       <c r="DP2" t="n">
-        <v>-0.0122990023591668</v>
-      </c>
-      <c r="DQ2"/>
+        <v>-601.887478358581</v>
+      </c>
+      <c r="DQ2" t="n">
+        <v>-655.277447730575</v>
+      </c>
       <c r="DR2" t="n">
-        <v>0.0118578424122401</v>
-      </c>
-      <c r="DS2"/>
-      <c r="DT2"/>
+        <v>255.169719676921</v>
+      </c>
+      <c r="DS2" t="n">
+        <v>-534.939188033917</v>
+      </c>
+      <c r="DT2" t="n">
+        <v>-355.556693015911</v>
+      </c>
       <c r="DU2" t="n">
-        <v>0.00423373735789115</v>
+        <v>227.982504358712</v>
       </c>
       <c r="DV2" t="n">
-        <v>-0.00205414744280956</v>
+        <v>-199.308480741729</v>
       </c>
       <c r="DW2" t="n">
-        <v>0.000408714782782181</v>
+        <v>116.971412145985</v>
       </c>
       <c r="DX2" t="n">
-        <v>0.00321012755637867</v>
+        <v>204.065018550283</v>
       </c>
       <c r="DY2" t="n">
-        <v>0.00485096659966935</v>
+        <v>197.759222385163</v>
       </c>
       <c r="DZ2" t="n">
-        <v>-0.00997287707281265</v>
-      </c>
-      <c r="EA2" t="n">
-        <v>-0.000218165248823758</v>
-      </c>
+        <v>-4.73464896585228</v>
+      </c>
+      <c r="EA2"/>
       <c r="EB2" t="n">
-        <v>0.000551340277322914</v>
-      </c>
-      <c r="EC2"/>
-      <c r="ED2" t="n">
-        <v>-0.00347339128967313</v>
-      </c>
-      <c r="EE2"/>
+        <v>-144.042952432229</v>
+      </c>
+      <c r="EC2" t="n">
+        <v>163.626138363074</v>
+      </c>
+      <c r="ED2"/>
+      <c r="EE2" t="n">
+        <v>57.0895819099619</v>
+      </c>
       <c r="EF2" t="n">
-        <v>0.0136249242800312</v>
-      </c>
-      <c r="EG2"/>
+        <v>-46.5139714935541</v>
+      </c>
+      <c r="EG2" t="n">
+        <v>224.703848455585</v>
+      </c>
       <c r="EH2" t="n">
-        <v>0.0022793872973777</v>
+        <v>-238.491821535875</v>
       </c>
       <c r="EI2" t="n">
-        <v>0.00158428263815852</v>
-      </c>
-      <c r="EJ2"/>
+        <v>196.712120573614</v>
+      </c>
+      <c r="EJ2" t="n">
+        <v>199.809777691515</v>
+      </c>
       <c r="EK2" t="n">
-        <v>0.0148941046820604</v>
+        <v>-3915.52272967454</v>
       </c>
       <c r="EL2" t="n">
-        <v>0.0130299989590248</v>
+        <v>185.811234915227</v>
       </c>
       <c r="EM2" t="n">
-        <v>0.001714630929229</v>
+        <v>-1564.80103092644</v>
       </c>
       <c r="EN2" t="n">
-        <v>0.00631057285234826</v>
+        <v>153.205812495172</v>
       </c>
       <c r="EO2" t="n">
-        <v>0</v>
+        <v>196.620951951001</v>
       </c>
       <c r="EP2" t="n">
-        <v>0.0112928448214244</v>
-      </c>
-      <c r="EQ2" t="n">
-        <v>0.000306592455004204</v>
-      </c>
+        <v>118.756331000429</v>
+      </c>
+      <c r="EQ2"/>
       <c r="ER2" t="n">
-        <v>-0.0103121841994999</v>
+        <v>170.726207926267</v>
       </c>
       <c r="ES2" t="n">
-        <v>-0.00523376878821256</v>
+        <v>-163.325595930992</v>
       </c>
       <c r="ET2" t="n">
-        <v>-0.00461662233276537</v>
+        <v>-241.605540378305</v>
       </c>
       <c r="EU2" t="n">
-        <v>0.000289396351640338</v>
+        <v>-810.107862367249</v>
       </c>
       <c r="EV2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EW2" t="n">
-        <v>0.0156906420238651</v>
-      </c>
+        <v>182.726001759872</v>
+      </c>
+      <c r="EW2"/>
       <c r="EX2" t="n">
-        <v>0.00427737927459854</v>
-      </c>
-      <c r="EY2"/>
+        <v>192.84362075354</v>
+      </c>
+      <c r="EY2" t="n">
+        <v>214.812653603885</v>
+      </c>
       <c r="EZ2" t="n">
-        <v>0.00543701416122187</v>
-      </c>
-      <c r="FA2"/>
+        <v>124.988431111307</v>
+      </c>
+      <c r="FA2" t="n">
+        <v>228.052001494068</v>
+      </c>
       <c r="FB2" t="n">
-        <v>0.00244177260296653</v>
-      </c>
-      <c r="FC2"/>
+        <v>93.4142640597317</v>
+      </c>
+      <c r="FC2" t="n">
+        <v>223.011586520781</v>
+      </c>
       <c r="FD2" t="n">
-        <v>0</v>
-      </c>
-      <c r="FE2"/>
-      <c r="FF2"/>
-      <c r="FG2" t="n">
-        <v>0.0064762855540297</v>
-      </c>
+        <v>-289.490171104686</v>
+      </c>
+      <c r="FE2" t="n">
+        <v>206.733308827961</v>
+      </c>
+      <c r="FF2" t="n">
+        <v>69.3449893348494</v>
+      </c>
+      <c r="FG2"/>
       <c r="FH2" t="n">
-        <v>0.0104949467258887</v>
+        <v>203.283037943749</v>
       </c>
       <c r="FI2" t="n">
-        <v>0</v>
+        <v>200.389667143952</v>
       </c>
       <c r="FJ2" t="n">
-        <v>-0.000536334110083664</v>
-      </c>
-      <c r="FK2"/>
+        <v>213.458735771433</v>
+      </c>
+      <c r="FK2" t="n">
+        <v>-153.3522359672</v>
+      </c>
       <c r="FL2" t="n">
-        <v>0</v>
+        <v>-1256.84772859951</v>
       </c>
       <c r="FM2" t="n">
-        <v>0.000831871945226889</v>
+        <v>226.239722625196</v>
       </c>
       <c r="FN2" t="n">
-        <v>0</v>
+        <v>191.266724746965</v>
       </c>
       <c r="FO2" t="n">
-        <v>0.0100872572897246</v>
+        <v>245.062183400689</v>
       </c>
       <c r="FP2" t="n">
-        <v>0.00360472029934705</v>
+        <v>138.808538433483</v>
       </c>
       <c r="FQ2" t="n">
-        <v>0.000112782239843026</v>
+        <v>173.883739737477</v>
       </c>
       <c r="FR2" t="n">
-        <v>0</v>
+        <v>225.520312798273</v>
       </c>
       <c r="FS2" t="n">
-        <v>0.00318834924369617</v>
+        <v>143.300669973747</v>
       </c>
       <c r="FT2" t="n">
-        <v>0.0000349231624274589</v>
+        <v>199.045278066756</v>
       </c>
       <c r="FU2" t="n">
-        <v>0</v>
+        <v>204.938181987822</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rights_proposed adjusted for footprint + manually
</commit_message>
<xml_diff>
--- a/xlsx/'folder' missing.xlsx
+++ b/xlsx/'folder' missing.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="177">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -218,9 +218,6 @@
     <t xml:space="preserve">Guyana</t>
   </si>
   <si>
-    <t xml:space="preserve">Hong Kong</t>
-  </si>
-  <si>
     <t xml:space="preserve">Honduras</t>
   </si>
   <si>
@@ -404,148 +401,148 @@
     <t xml:space="preserve">Poland</t>
   </si>
   <si>
+    <t xml:space="preserve">Portugal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paraguay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qatar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Romania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Russia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rwanda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saudi Arabia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sudan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Senegal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Singapore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solomon Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sierra Leone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Salvador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Somalia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serbia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Sudan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suriname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slovakia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slovenia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swaziland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Syria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Togo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thailand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tajikistan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turkmenistan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trinidad and Tobago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tunisia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turkey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taiwan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tanzania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uganda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ukraine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uruguay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uzbekistan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venezuela</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vietnam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vanuatu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samoa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yemen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Africa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zambia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zimbabwe</t>
+  </si>
+  <si>
     <t xml:space="preserve">North Korea</t>
   </si>
   <si>
-    <t xml:space="preserve">Portugal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paraguay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Qatar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Romania</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Russia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rwanda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saudi Arabia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sudan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Senegal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Singapore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solomon Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sierra Leone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El Salvador</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Somalia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serbia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South Sudan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suriname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slovakia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slovenia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sweden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Swaziland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Syria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Togo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thailand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tajikistan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Turkmenistan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Timor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trinidad and Tobago</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tunisia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Turkey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taiwan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tanzania</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uganda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ukraine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uruguay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uzbekistan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Venezuela</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vietnam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vanuatu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Samoa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yemen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South Africa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zambia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zimbabwe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">budget_gain_over_gdp_both_taxes_pop</t>
+    <t xml:space="preserve">diff_npv_ede_ffu_nl</t>
   </si>
 </sst>
 </file>
@@ -1406,534 +1403,186 @@
       <c r="FT1" t="s">
         <v>175</v>
       </c>
-      <c r="FU1" t="s">
-        <v>176</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0.476856873993071</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.107397031561235</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.0327123332353865</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.0334231630277939</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.024678643551008</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.0354238889054595</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.0246949431148153</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.0152445767360406</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.0420214111994607</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.802503861274238</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0.0148565181786644</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0.132369270903566</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0.207811246319691</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0.0638850152856799</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0.0249199157937318</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>0.025576749670401</v>
-      </c>
-      <c r="R2" t="n">
-        <v>0.0127191067193463</v>
-      </c>
-      <c r="S2" t="n">
-        <v>0.037186467070477</v>
-      </c>
-      <c r="T2" t="n">
-        <v>0.041594443442989</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0.033605621530454</v>
-      </c>
-      <c r="V2" t="n">
-        <v>0.0629348926575691</v>
-      </c>
-      <c r="W2" t="n">
-        <v>0.0358703420909474</v>
-      </c>
-      <c r="X2" t="n">
-        <v>0.0131250094065487</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>0.0222380464882366</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>0.0657780460343649</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>0.0283693555709704</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>0.322510916783072</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>0.0242738797967521</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>0.0296255006294935</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>0.0215972902297294</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>0.0343423693905308</v>
-      </c>
-      <c r="AG2" t="n">
-        <v>0.0758317202601664</v>
-      </c>
-      <c r="AH2" t="n">
-        <v>0.111177406264219</v>
-      </c>
-      <c r="AI2" t="n">
-        <v>0.270024924638564</v>
-      </c>
-      <c r="AJ2" t="n">
-        <v>0.10300042968212</v>
-      </c>
-      <c r="AK2" t="n">
-        <v>0.040746577493648</v>
-      </c>
-      <c r="AL2" t="n">
-        <v>0.118064279404514</v>
-      </c>
-      <c r="AM2" t="n">
-        <v>0.0456098508174919</v>
-      </c>
-      <c r="AN2" t="n">
-        <v>0.0208502248328664</v>
-      </c>
-      <c r="AO2" t="n">
-        <v>0.134923699176072</v>
-      </c>
-      <c r="AP2" t="n">
-        <v>0.014925002934785</v>
-      </c>
-      <c r="AQ2" t="n">
-        <v>0.0126303516280692</v>
-      </c>
-      <c r="AR2" t="n">
-        <v>0.0154164157852496</v>
-      </c>
-      <c r="AS2" t="n">
-        <v>0.0597568963975836</v>
-      </c>
-      <c r="AT2" t="n">
-        <v>0.0220462650937407</v>
-      </c>
-      <c r="AU2" t="n">
-        <v>0.0232280472613901</v>
-      </c>
-      <c r="AV2" t="n">
-        <v>0.0510471548630055</v>
-      </c>
-      <c r="AW2" t="n">
-        <v>0.0387186476046751</v>
-      </c>
-      <c r="AX2" t="n">
-        <v>0.0573751280969474</v>
-      </c>
-      <c r="AY2" t="n">
-        <v>0.288660704100691</v>
-      </c>
-      <c r="AZ2" t="n">
-        <v>0.0108819379435483</v>
-      </c>
-      <c r="BA2" t="n">
-        <v>0.0227496563925462</v>
-      </c>
-      <c r="BB2" t="n">
-        <v>0.167019162920659</v>
-      </c>
-      <c r="BC2" t="n">
-        <v>0.00836560363930897</v>
-      </c>
-      <c r="BD2" t="n">
-        <v>0.0626916128569344</v>
-      </c>
-      <c r="BE2" t="n">
-        <v>0.0233710050495614</v>
-      </c>
-      <c r="BF2" t="n">
-        <v>0.0416174979942574</v>
-      </c>
-      <c r="BG2" t="n">
-        <v>0.0321813441834787</v>
-      </c>
-      <c r="BH2" t="n">
-        <v>0.0407242126741012</v>
-      </c>
-      <c r="BI2" t="n">
-        <v>0.0856757128903284</v>
-      </c>
-      <c r="BJ2" t="n">
-        <v>0.174686554822661</v>
-      </c>
-      <c r="BK2" t="n">
-        <v>0.208837505017312</v>
-      </c>
-      <c r="BL2" t="n">
-        <v>0.19737442681269</v>
-      </c>
-      <c r="BM2" t="n">
-        <v>0.0863633281968772</v>
-      </c>
-      <c r="BN2" t="n">
-        <v>0.0252760616235968</v>
-      </c>
-      <c r="BO2" t="n">
-        <v>0.0376407848931566</v>
-      </c>
-      <c r="BP2" t="n">
-        <v>0.0186584190680676</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2"/>
+      <c r="Y2"/>
+      <c r="Z2"/>
+      <c r="AA2"/>
+      <c r="AB2"/>
+      <c r="AC2"/>
+      <c r="AD2"/>
+      <c r="AE2"/>
+      <c r="AF2"/>
+      <c r="AG2"/>
+      <c r="AH2"/>
+      <c r="AI2"/>
+      <c r="AJ2"/>
+      <c r="AK2"/>
+      <c r="AL2"/>
+      <c r="AM2"/>
+      <c r="AN2"/>
+      <c r="AO2"/>
+      <c r="AP2"/>
+      <c r="AQ2"/>
+      <c r="AR2"/>
+      <c r="AS2"/>
+      <c r="AT2"/>
+      <c r="AU2"/>
+      <c r="AV2"/>
+      <c r="AW2"/>
+      <c r="AX2"/>
+      <c r="AY2"/>
+      <c r="AZ2"/>
+      <c r="BA2"/>
+      <c r="BB2"/>
+      <c r="BC2"/>
+      <c r="BD2"/>
+      <c r="BE2"/>
+      <c r="BF2"/>
+      <c r="BG2"/>
+      <c r="BH2"/>
+      <c r="BI2"/>
+      <c r="BJ2"/>
+      <c r="BK2"/>
+      <c r="BL2"/>
+      <c r="BM2"/>
+      <c r="BN2"/>
+      <c r="BO2"/>
+      <c r="BP2"/>
       <c r="BQ2"/>
-      <c r="BR2" t="n">
-        <v>0.0723452000833387</v>
-      </c>
-      <c r="BS2" t="n">
-        <v>0.0170406403709969</v>
-      </c>
-      <c r="BT2" t="n">
-        <v>0.111781664525451</v>
-      </c>
-      <c r="BU2" t="n">
-        <v>0.0149336727411018</v>
-      </c>
-      <c r="BV2" t="n">
-        <v>0.0489809391767009</v>
-      </c>
-      <c r="BW2" t="n">
-        <v>0.10178653028816</v>
-      </c>
-      <c r="BX2" t="n">
-        <v>0.0236139570281611</v>
-      </c>
-      <c r="BY2" t="n">
-        <v>0.0692299294762357</v>
-      </c>
-      <c r="BZ2" t="n">
-        <v>0.0581733795093361</v>
-      </c>
-      <c r="CA2" t="n">
-        <v>0.0300666019472384</v>
-      </c>
-      <c r="CB2" t="n">
-        <v>0.017291518579654</v>
-      </c>
-      <c r="CC2" t="n">
-        <v>0.00813497008101037</v>
-      </c>
-      <c r="CD2" t="n">
-        <v>0.0426688161419081</v>
-      </c>
-      <c r="CE2" t="n">
-        <v>0.0559500990666387</v>
-      </c>
-      <c r="CF2" t="n">
-        <v>0.0113634867337095</v>
-      </c>
-      <c r="CG2" t="n">
-        <v>0.0374367731268203</v>
-      </c>
-      <c r="CH2" t="n">
-        <v>0.0918745083433875</v>
-      </c>
-      <c r="CI2" t="n">
-        <v>0.124017718308494</v>
-      </c>
-      <c r="CJ2" t="n">
-        <v>0.0895524017383139</v>
-      </c>
-      <c r="CK2" t="n">
-        <v>0.0128535627028676</v>
-      </c>
-      <c r="CL2" t="n">
-        <v>0.023243312055857</v>
-      </c>
-      <c r="CM2" t="n">
-        <v>0.0965448942151482</v>
-      </c>
-      <c r="CN2" t="n">
-        <v>0.0652278912461664</v>
-      </c>
-      <c r="CO2" t="n">
-        <v>0.274791436825517</v>
-      </c>
-      <c r="CP2" t="n">
-        <v>0.0523450048113142</v>
-      </c>
-      <c r="CQ2" t="n">
-        <v>0.0692677054421867</v>
-      </c>
-      <c r="CR2" t="n">
-        <v>0.165368721879093</v>
-      </c>
-      <c r="CS2" t="n">
-        <v>0.0151821677897138</v>
-      </c>
-      <c r="CT2" t="n">
-        <v>0.0942965455407739</v>
-      </c>
-      <c r="CU2" t="n">
-        <v>0.02272509445252</v>
-      </c>
-      <c r="CV2" t="n">
-        <v>0.0652611357175624</v>
-      </c>
-      <c r="CW2" t="n">
-        <v>0.0406205322008383</v>
-      </c>
-      <c r="CX2" t="n">
-        <v>0.365619258008749</v>
-      </c>
-      <c r="CY2" t="n">
-        <v>0.0222220853816657</v>
-      </c>
-      <c r="CZ2" t="n">
-        <v>0.0228657405077065</v>
-      </c>
-      <c r="DA2" t="n">
-        <v>0.0351043518414059</v>
-      </c>
-      <c r="DB2" t="n">
-        <v>0.20681867125672</v>
-      </c>
-      <c r="DC2" t="n">
-        <v>0.0244501523882075</v>
-      </c>
-      <c r="DD2" t="n">
-        <v>0.176827306536459</v>
-      </c>
-      <c r="DE2" t="n">
-        <v>0.0242205983737763</v>
-      </c>
-      <c r="DF2" t="n">
-        <v>0.0562425457738618</v>
-      </c>
-      <c r="DG2" t="n">
-        <v>0.351499411721486</v>
-      </c>
-      <c r="DH2" t="n">
-        <v>0.116529795439902</v>
-      </c>
-      <c r="DI2" t="n">
-        <v>0.0400930414298921</v>
-      </c>
-      <c r="DJ2" t="n">
-        <v>0.29934283713796</v>
-      </c>
-      <c r="DK2" t="n">
-        <v>0.0376237371465732</v>
-      </c>
-      <c r="DL2" t="n">
-        <v>0.055460925309362</v>
-      </c>
-      <c r="DM2" t="n">
-        <v>0.272947099699755</v>
-      </c>
-      <c r="DN2" t="n">
-        <v>0.0988181932916351</v>
-      </c>
-      <c r="DO2" t="n">
-        <v>0.089931980383748</v>
-      </c>
-      <c r="DP2" t="n">
-        <v>0.0111704093129657</v>
-      </c>
-      <c r="DQ2" t="n">
-        <v>0.00526257938364951</v>
-      </c>
-      <c r="DR2" t="n">
-        <v>0.144127568903385</v>
-      </c>
-      <c r="DS2" t="n">
-        <v>0.0211803288521644</v>
-      </c>
-      <c r="DT2" t="n">
-        <v>0.0310436397625985</v>
-      </c>
-      <c r="DU2" t="n">
-        <v>0.128081707944893</v>
-      </c>
-      <c r="DV2" t="n">
-        <v>0.0232267019967182</v>
-      </c>
-      <c r="DW2" t="n">
-        <v>0.0391798231196298</v>
-      </c>
-      <c r="DX2" t="n">
-        <v>0.0476178852222121</v>
-      </c>
-      <c r="DY2" t="n">
-        <v>0.0752771462496949</v>
-      </c>
-      <c r="DZ2" t="n">
-        <v>0.0144785849562027</v>
-      </c>
+      <c r="BR2"/>
+      <c r="BS2"/>
+      <c r="BT2"/>
+      <c r="BU2"/>
+      <c r="BV2"/>
+      <c r="BW2"/>
+      <c r="BX2"/>
+      <c r="BY2"/>
+      <c r="BZ2"/>
+      <c r="CA2"/>
+      <c r="CB2"/>
+      <c r="CC2"/>
+      <c r="CD2"/>
+      <c r="CE2"/>
+      <c r="CF2"/>
+      <c r="CG2"/>
+      <c r="CH2"/>
+      <c r="CI2"/>
+      <c r="CJ2"/>
+      <c r="CK2"/>
+      <c r="CL2"/>
+      <c r="CM2"/>
+      <c r="CN2"/>
+      <c r="CO2"/>
+      <c r="CP2"/>
+      <c r="CQ2"/>
+      <c r="CR2"/>
+      <c r="CS2"/>
+      <c r="CT2"/>
+      <c r="CU2"/>
+      <c r="CV2"/>
+      <c r="CW2"/>
+      <c r="CX2"/>
+      <c r="CY2"/>
+      <c r="CZ2"/>
+      <c r="DA2"/>
+      <c r="DB2"/>
+      <c r="DC2"/>
+      <c r="DD2"/>
+      <c r="DE2"/>
+      <c r="DF2"/>
+      <c r="DG2"/>
+      <c r="DH2"/>
+      <c r="DI2"/>
+      <c r="DJ2"/>
+      <c r="DK2"/>
+      <c r="DL2"/>
+      <c r="DM2"/>
+      <c r="DN2"/>
+      <c r="DO2"/>
+      <c r="DP2"/>
+      <c r="DQ2"/>
+      <c r="DR2"/>
+      <c r="DS2"/>
+      <c r="DT2"/>
+      <c r="DU2"/>
+      <c r="DV2"/>
+      <c r="DW2"/>
+      <c r="DX2"/>
+      <c r="DY2"/>
+      <c r="DZ2"/>
       <c r="EA2"/>
-      <c r="EB2" t="n">
-        <v>0.0116657657074069</v>
-      </c>
-      <c r="EC2" t="n">
-        <v>0.0353500308390415</v>
-      </c>
-      <c r="ED2" t="n">
-        <v>0.0310963454961043</v>
-      </c>
-      <c r="EE2" t="n">
-        <v>0.00958918310702964</v>
-      </c>
-      <c r="EF2" t="n">
-        <v>0.0314707353401105</v>
-      </c>
-      <c r="EG2" t="n">
-        <v>0.188464628721927</v>
-      </c>
-      <c r="EH2" t="n">
-        <v>0.0117979955280415</v>
-      </c>
-      <c r="EI2" t="n">
-        <v>0.214433309553778</v>
-      </c>
-      <c r="EJ2" t="n">
-        <v>0.114976445009324</v>
-      </c>
-      <c r="EK2" t="n">
-        <v>0.0559687161532934</v>
-      </c>
-      <c r="EL2" t="n">
-        <v>0.0971891226178407</v>
-      </c>
-      <c r="EM2" t="n">
-        <v>7.61424935486216</v>
-      </c>
-      <c r="EN2" t="n">
-        <v>0.0536011783632085</v>
-      </c>
-      <c r="EO2" t="n">
-        <v>0.290742922328</v>
-      </c>
-      <c r="EP2" t="n">
-        <v>0.0275491263646958</v>
-      </c>
+      <c r="EB2"/>
+      <c r="EC2"/>
+      <c r="ED2"/>
+      <c r="EE2"/>
+      <c r="EF2"/>
+      <c r="EG2"/>
+      <c r="EH2"/>
+      <c r="EI2"/>
+      <c r="EJ2"/>
+      <c r="EK2"/>
+      <c r="EL2"/>
+      <c r="EM2"/>
+      <c r="EN2"/>
+      <c r="EO2"/>
+      <c r="EP2"/>
       <c r="EQ2"/>
-      <c r="ER2" t="n">
-        <v>0.0594317194559274</v>
-      </c>
-      <c r="ES2" t="n">
-        <v>0.0162148725795203</v>
-      </c>
-      <c r="ET2" t="n">
-        <v>0.0136701290396092</v>
-      </c>
-      <c r="EU2" t="n">
-        <v>0.0184242620852437</v>
-      </c>
-      <c r="EV2" t="n">
-        <v>0.0568169302650267</v>
-      </c>
-      <c r="EW2" t="n">
-        <v>0.314401321038932</v>
-      </c>
-      <c r="EX2" t="n">
-        <v>0.258395376185435</v>
-      </c>
-      <c r="EY2" t="n">
-        <v>0.191467066612336</v>
-      </c>
-      <c r="EZ2" t="n">
-        <v>0.0478986872620342</v>
-      </c>
-      <c r="FA2" t="n">
-        <v>0.141039094503463</v>
-      </c>
-      <c r="FB2" t="n">
-        <v>0.0413899728167516</v>
-      </c>
-      <c r="FC2" t="n">
-        <v>0.0980818034875118</v>
-      </c>
-      <c r="FD2" t="n">
-        <v>0.0464745691705364</v>
-      </c>
-      <c r="FE2" t="n">
-        <v>0.0667298123626552</v>
-      </c>
-      <c r="FF2" t="n">
-        <v>0.0198649400938047</v>
-      </c>
+      <c r="ER2"/>
+      <c r="ES2"/>
+      <c r="ET2"/>
+      <c r="EU2"/>
+      <c r="EV2"/>
+      <c r="EW2"/>
+      <c r="EX2"/>
+      <c r="EY2"/>
+      <c r="EZ2"/>
+      <c r="FA2"/>
+      <c r="FB2"/>
+      <c r="FC2"/>
+      <c r="FD2"/>
+      <c r="FE2"/>
+      <c r="FF2"/>
       <c r="FG2"/>
-      <c r="FH2" t="n">
-        <v>0.146538355958246</v>
-      </c>
-      <c r="FI2" t="n">
-        <v>0.181108023915719</v>
-      </c>
-      <c r="FJ2" t="n">
-        <v>0.0606433399644432</v>
-      </c>
-      <c r="FK2" t="n">
-        <v>0.0162798738803285</v>
-      </c>
-      <c r="FL2" t="n">
-        <v>0.0259181302285738</v>
-      </c>
-      <c r="FM2" t="n">
-        <v>0.0883036950122291</v>
-      </c>
-      <c r="FN2" t="n">
-        <v>0.0230120253756278</v>
-      </c>
-      <c r="FO2" t="n">
-        <v>0.0571672142623785</v>
-      </c>
-      <c r="FP2" t="n">
-        <v>0.0607817384751831</v>
-      </c>
-      <c r="FQ2" t="n">
-        <v>0.046885015828484</v>
-      </c>
-      <c r="FR2" t="n">
-        <v>0.265848431494365</v>
-      </c>
-      <c r="FS2" t="n">
-        <v>0.0588806445311511</v>
-      </c>
-      <c r="FT2" t="n">
-        <v>0.142066640691575</v>
-      </c>
-      <c r="FU2" t="n">
-        <v>0.0920664746438403</v>
-      </c>
+      <c r="FH2"/>
+      <c r="FI2"/>
+      <c r="FJ2"/>
+      <c r="FK2"/>
+      <c r="FL2"/>
+      <c r="FM2"/>
+      <c r="FN2"/>
+      <c r="FO2"/>
+      <c r="FP2"/>
+      <c r="FQ2"/>
+      <c r="FR2"/>
+      <c r="FS2"/>
+      <c r="FT2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
manual_adjust post fix sum transfer
</commit_message>
<xml_diff>
--- a/xlsx/'folder' missing.xlsx
+++ b/xlsx/'folder' missing.xlsx
@@ -449,7 +449,7 @@
     <t xml:space="preserve">Zimbabwe</t>
   </si>
   <si>
-    <t xml:space="preserve">var_npv_ede_ffu_nl</t>
+    <t xml:space="preserve">mean_transfer_over_gdp</t>
   </si>
 </sst>
 </file>
@@ -1223,436 +1223,436 @@
         <v>145</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0685271540660919</v>
+        <v>0.0413938306792532</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0383727285495903</v>
+        <v>0.0141816551975709</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0116830580021328</v>
+        <v>0.00946516095329444</v>
       </c>
       <c r="E2" t="n">
-        <v>0.00105359962828633</v>
+        <v>0.0000951480991964588</v>
       </c>
       <c r="F2" t="n">
-        <v>0.00846987956327538</v>
+        <v>0.00570157453184357</v>
       </c>
       <c r="G2" t="n">
-        <v>0.00755896571618675</v>
+        <v>-0.00558446480532269</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0815211020559163</v>
+        <v>0.0466764060485216</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0206027434757696</v>
+        <v>-0.0117502348337724</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0312640253278136</v>
+        <v>0.0110454972958553</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0428851625633972</v>
+        <v>0.0201651903787048</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0134609216819188</v>
+        <v>0.00909981356802385</v>
       </c>
       <c r="M2" t="n">
-        <v>0.00428950894132907</v>
+        <v>-0.000614566868231799</v>
       </c>
       <c r="N2" t="n">
-        <v>0.000223418008657328</v>
+        <v>0.000596282677563316</v>
       </c>
       <c r="O2" t="n">
-        <v>0.00436153451111543</v>
+        <v>-0.0090000876383852</v>
       </c>
       <c r="P2" t="n">
-        <v>0.0401576554286707</v>
+        <v>0.00975849017381169</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.00434172931039423</v>
+        <v>0.00201405372162403</v>
       </c>
       <c r="R2" t="n">
-        <v>0.0414931919964285</v>
+        <v>0.00707880875164765</v>
       </c>
       <c r="S2" t="n">
-        <v>0.0086867765015044</v>
+        <v>0.00440608485326436</v>
       </c>
       <c r="T2" t="n">
-        <v>0.00335666270645185</v>
+        <v>0.0000697596300239161</v>
       </c>
       <c r="U2" t="n">
-        <v>-0.00141409861666542</v>
+        <v>0.00279507500689928</v>
       </c>
       <c r="V2" t="n">
-        <v>0.297107975116057</v>
+        <v>0.0540020919258936</v>
       </c>
       <c r="W2" t="n">
-        <v>0.0194836925530693</v>
+        <v>-0.00938714470721567</v>
       </c>
       <c r="X2" t="n">
-        <v>0.00373833837208504</v>
+        <v>-0.000906456666114651</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.00737049766439957</v>
+        <v>-0.00695717879217674</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.00282013204622844</v>
+        <v>0.00318292080179674</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.029613596298941</v>
+        <v>0.0122116098361174</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.0526303565058748</v>
+        <v>0.0244086955570301</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.0256325462981901</v>
+        <v>0.0115402027407016</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.0282726542350844</v>
+        <v>0.00561471468871215</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.118403528852998</v>
+        <v>0.019851765516985</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.0401832995247262</v>
+        <v>0.010803810441459</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.0029211543154779</v>
+        <v>0.00403852327272275</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.0108308059680022</v>
+        <v>0.00925337714862955</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.000336375593958049</v>
+        <v>0.00108322795466306</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.00330663625815131</v>
+        <v>-0.00500658095829559</v>
       </c>
       <c r="AK2" t="n">
-        <v>0.00728874328294848</v>
+        <v>-0.00587626998158726</v>
       </c>
       <c r="AL2" t="n">
-        <v>0.0461114927421569</v>
+        <v>0.0154741353681295</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.00806935843019674</v>
+        <v>-0.00451588879885965</v>
       </c>
       <c r="AN2" t="n">
-        <v>0.0096824892976628</v>
+        <v>0.00225786505456608</v>
       </c>
       <c r="AO2" t="n">
-        <v>0.00310110939488339</v>
+        <v>-0.000600497116212502</v>
       </c>
       <c r="AP2" t="n">
-        <v>0.00246828534517318</v>
+        <v>0.00154689264000408</v>
       </c>
       <c r="AQ2" t="n">
-        <v>-0.000903396551021673</v>
+        <v>-0.000233546381607169</v>
       </c>
       <c r="AR2" t="n">
-        <v>0.355208627832584</v>
+        <v>0.126207069066058</v>
       </c>
       <c r="AS2" t="n">
-        <v>0.00330129698480031</v>
+        <v>-0.00401873659003747</v>
       </c>
       <c r="AT2" t="n">
-        <v>0.00626742078253195</v>
+        <v>-0.0078412996344824</v>
       </c>
       <c r="AU2" t="n">
-        <v>0.0287343574951873</v>
+        <v>0.017336762032432</v>
       </c>
       <c r="AV2" t="n">
-        <v>0.0101292502538097</v>
+        <v>-0.00635801641070753</v>
       </c>
       <c r="AW2" t="n">
-        <v>0.00539557825986581</v>
+        <v>-0.00406078344217508</v>
       </c>
       <c r="AX2" t="n">
-        <v>0.00700968893483545</v>
+        <v>0.00352505633088435</v>
       </c>
       <c r="AY2" t="n">
-        <v>0.00779931101513864</v>
+        <v>-0.00524855333424494</v>
       </c>
       <c r="AZ2" t="n">
-        <v>0.00302780158921467</v>
+        <v>0.0000289666060314453</v>
       </c>
       <c r="BA2" t="n">
-        <v>0.0293556105086294</v>
+        <v>0.0118990747943195</v>
       </c>
       <c r="BB2" t="n">
-        <v>0.0238968362909746</v>
+        <v>0.0141833634476714</v>
       </c>
       <c r="BC2" t="n">
-        <v>0.074275316143535</v>
+        <v>0.0206760931891854</v>
       </c>
       <c r="BD2" t="n">
-        <v>0.0781624725623766</v>
+        <v>0.0193347431369358</v>
       </c>
       <c r="BE2" t="n">
-        <v>0.00176616961577181</v>
+        <v>0.000818420431837212</v>
       </c>
       <c r="BF2" t="n">
-        <v>0.000388431074406226</v>
+        <v>-0.00491683176873893</v>
       </c>
       <c r="BG2" t="n">
-        <v>0.0116582380664734</v>
+        <v>0.00519281975663479</v>
       </c>
       <c r="BH2" t="n">
-        <v>0.00476495196396143</v>
+        <v>0.00318990704348918</v>
       </c>
       <c r="BI2" t="n">
-        <v>0.0531170170301298</v>
+        <v>0.0106347377438979</v>
       </c>
       <c r="BJ2" t="n">
-        <v>0.00335068830245655</v>
+        <v>0.00266474871843922</v>
       </c>
       <c r="BK2" t="n">
-        <v>0.1469850200543</v>
+        <v>0.0271336846630891</v>
       </c>
       <c r="BL2" t="n">
-        <v>0.00735279675464717</v>
+        <v>-0.00603801781059794</v>
       </c>
       <c r="BM2" t="n">
-        <v>-0.000515411100244889</v>
+        <v>-0.000268201758402401</v>
       </c>
       <c r="BN2" t="n">
-        <v>0.0109949010531698</v>
+        <v>0.0030050304162045</v>
       </c>
       <c r="BO2" t="n">
-        <v>0.00414538912447049</v>
+        <v>-0.00282755398221118</v>
       </c>
       <c r="BP2" t="n">
-        <v>0.00699941147434413</v>
+        <v>-0.00950535657251373</v>
       </c>
       <c r="BQ2" t="n">
-        <v>0.00432915298817682</v>
+        <v>-0.00543362439791557</v>
       </c>
       <c r="BR2" t="n">
-        <v>0.0070187809940625</v>
+        <v>-0.00670007859783028</v>
       </c>
       <c r="BS2" t="n">
-        <v>0.00435683083180294</v>
+        <v>-0.00477957394433243</v>
       </c>
       <c r="BT2" t="n">
-        <v>0.061399070659601</v>
+        <v>0.00897559131079077</v>
       </c>
       <c r="BU2" t="n">
-        <v>-0.000584795650812819</v>
+        <v>-0.000962947433063889</v>
       </c>
       <c r="BV2" t="n">
-        <v>0.00908131543496538</v>
+        <v>-0.0024773543506846</v>
       </c>
       <c r="BW2" t="n">
-        <v>0.0581284390574919</v>
+        <v>0.015064405996304</v>
       </c>
       <c r="BX2" t="n">
-        <v>0.00244832555738994</v>
+        <v>-0.00102448425189035</v>
       </c>
       <c r="BY2" t="n">
-        <v>0.0149835762743455</v>
+        <v>-0.00929553248775824</v>
       </c>
       <c r="BZ2" t="n">
-        <v>-0.000453124005781569</v>
+        <v>-0.00984292562693678</v>
       </c>
       <c r="CA2" t="n">
-        <v>0.0680596572368899</v>
+        <v>0.0362906630147998</v>
       </c>
       <c r="CB2" t="n">
-        <v>0.00142673593949372</v>
+        <v>-0.00193661000946414</v>
       </c>
       <c r="CC2" t="n">
-        <v>0.000690690542401118</v>
+        <v>0.00176802813629976</v>
       </c>
       <c r="CD2" t="n">
-        <v>0.098935482111743</v>
+        <v>0.0175641219813685</v>
       </c>
       <c r="CE2" t="n">
-        <v>0.0090159830329648</v>
+        <v>-0.00620934815514835</v>
       </c>
       <c r="CF2" t="n">
-        <v>0.00664883089231783</v>
+        <v>-0.00518009841146406</v>
       </c>
       <c r="CG2" t="n">
-        <v>0.0148211910482094</v>
+        <v>-0.00886440422467589</v>
       </c>
       <c r="CH2" t="n">
-        <v>0.00633584359088646</v>
+        <v>0.00123563251979544</v>
       </c>
       <c r="CI2" t="n">
-        <v>0.00526014372239469</v>
+        <v>-0.0041397522227783</v>
       </c>
       <c r="CJ2" t="n">
-        <v>0.0591890550055723</v>
+        <v>0.0265627884023923</v>
       </c>
       <c r="CK2" t="n">
-        <v>0.000283525347884117</v>
+        <v>0.000556142824684237</v>
       </c>
       <c r="CL2" t="n">
-        <v>0.000630858872544993</v>
+        <v>0.000373370310322225</v>
       </c>
       <c r="CM2" t="n">
-        <v>0.0375200589555753</v>
+        <v>0.0218207436079144</v>
       </c>
       <c r="CN2" t="n">
-        <v>0.0306525688386328</v>
+        <v>-0.0127230324997295</v>
       </c>
       <c r="CO2" t="n">
-        <v>0.0404063738506133</v>
+        <v>0.0190793745517016</v>
       </c>
       <c r="CP2" t="n">
-        <v>0.0152629589714586</v>
+        <v>-0.0470765908001615</v>
       </c>
       <c r="CQ2" t="n">
-        <v>0.0782899021844752</v>
+        <v>0.024122335582292</v>
       </c>
       <c r="CR2" t="n">
-        <v>0.0146295296037722</v>
+        <v>0.00820554873850347</v>
       </c>
       <c r="CS2" t="n">
-        <v>0.00480739317043732</v>
+        <v>0.00411233350432648</v>
       </c>
       <c r="CT2" t="n">
-        <v>0.144462106515119</v>
+        <v>0.0444877632232503</v>
       </c>
       <c r="CU2" t="n">
-        <v>-0.0000115527313808705</v>
+        <v>-0.00308437358337995</v>
       </c>
       <c r="CV2" t="n">
-        <v>0.00123879502883839</v>
+        <v>0.00248851482897805</v>
       </c>
       <c r="CW2" t="n">
-        <v>0.0531899570573153</v>
+        <v>0.0337354487010322</v>
       </c>
       <c r="CX2" t="n">
-        <v>0.022819819539486</v>
+        <v>0.00985667921352351</v>
       </c>
       <c r="CY2" t="n">
-        <v>0.0124780011255556</v>
+        <v>0.00612261163841476</v>
       </c>
       <c r="CZ2" t="n">
-        <v>0.00791336278481869</v>
+        <v>-0.00586034852731582</v>
       </c>
       <c r="DA2" t="n">
-        <v>0.00512443910307558</v>
+        <v>-0.00445129181313277</v>
       </c>
       <c r="DB2" t="n">
-        <v>0.0273436114961283</v>
+        <v>0.0148199127783998</v>
       </c>
       <c r="DC2" t="n">
-        <v>0.00796343614149464</v>
+        <v>0.00493873512489233</v>
       </c>
       <c r="DD2" t="n">
-        <v>-0.00254818429992043</v>
+        <v>0.00116064989934569</v>
       </c>
       <c r="DE2" t="n">
-        <v>0.0110939399259153</v>
+        <v>0.00304186596491245</v>
       </c>
       <c r="DF2" t="n">
-        <v>0.00751872206514248</v>
+        <v>0.00388963246416255</v>
       </c>
       <c r="DG2" t="n">
-        <v>0.0304174406311173</v>
+        <v>0.00837324206125399</v>
       </c>
       <c r="DH2" t="n">
-        <v>0.0045234608310738</v>
+        <v>-0.00268143860403829</v>
       </c>
       <c r="DI2" t="n">
-        <v>0.00349054889725653</v>
+        <v>-0.00441264506610488</v>
       </c>
       <c r="DJ2" t="n">
-        <v>0.00337812961471684</v>
+        <v>0.00168510515869718</v>
       </c>
       <c r="DK2" t="n">
-        <v>0.00243952672424474</v>
+        <v>0.00144328622335737</v>
       </c>
       <c r="DL2" t="n">
-        <v>0.108802564595635</v>
+        <v>0.0253838478729565</v>
       </c>
       <c r="DM2" t="n">
-        <v>0.00439487852367249</v>
+        <v>0.00549058552739496</v>
       </c>
       <c r="DN2" t="n">
-        <v>0.0235016741332703</v>
+        <v>0.0108974049950124</v>
       </c>
       <c r="DO2" t="n">
-        <v>-0.00816095010642148</v>
+        <v>-0.00867154915547672</v>
       </c>
       <c r="DP2" t="n">
-        <v>0.0662928021296003</v>
+        <v>0.035386186290345</v>
       </c>
       <c r="DQ2" t="n">
-        <v>0.0239711181105442</v>
+        <v>0.0133581836310892</v>
       </c>
       <c r="DR2" t="n">
-        <v>0.00331777975143721</v>
+        <v>-0.00397936067700838</v>
       </c>
       <c r="DS2" t="n">
-        <v>0.00513469812168355</v>
+        <v>-0.00153202620773999</v>
       </c>
       <c r="DT2" t="n">
-        <v>0.00247629724060294</v>
+        <v>-0.00189172803418685</v>
       </c>
       <c r="DU2" t="n">
-        <v>0.00217194627436035</v>
+        <v>-0.00369209911200715</v>
       </c>
       <c r="DV2" t="n">
-        <v>0.00782536594856076</v>
+        <v>-0.0039116880717559</v>
       </c>
       <c r="DW2" t="n">
-        <v>0.0346324655990184</v>
+        <v>0.00799742707693966</v>
       </c>
       <c r="DX2" t="n">
-        <v>0.00713537910393036</v>
+        <v>0.00227001630721897</v>
       </c>
       <c r="DY2" t="n">
-        <v>0.0798127644557469</v>
+        <v>0.0298743651470338</v>
       </c>
       <c r="DZ2" t="n">
-        <v>0.0323834685063038</v>
+        <v>0.00887485960809664</v>
       </c>
       <c r="EA2" t="n">
-        <v>-0.00179092881653087</v>
+        <v>-0.000735188787234849</v>
       </c>
       <c r="EB2" t="n">
-        <v>0.0064118947399463</v>
+        <v>-0.0152771608710901</v>
       </c>
       <c r="EC2" t="n">
-        <v>0.0244483023693898</v>
+        <v>0.0142548253190453</v>
       </c>
       <c r="ED2" t="n">
-        <v>0.0072199251131988</v>
+        <v>0.00383363549703493</v>
       </c>
       <c r="EE2" t="n">
-        <v>0.0012519080131459</v>
+        <v>-0.00197227514491281</v>
       </c>
       <c r="EF2" t="n">
-        <v>0.0339665513702003</v>
+        <v>0.0169875835668753</v>
       </c>
       <c r="EG2" t="n">
-        <v>0.0638336213405439</v>
+        <v>0.0247565183559394</v>
       </c>
       <c r="EH2" t="n">
-        <v>0.00180377391226116</v>
+        <v>-0.00687259229937567</v>
       </c>
       <c r="EI2" t="n">
-        <v>0.00239252367383735</v>
+        <v>0.00223217824763678</v>
       </c>
       <c r="EJ2" t="n">
-        <v>0.0013278521749982</v>
+        <v>-0.00242635687211382</v>
       </c>
       <c r="EK2" t="n">
-        <v>0.00781141234361726</v>
+        <v>0.00274728260881245</v>
       </c>
       <c r="EL2" t="n">
-        <v>0.0850384735936947</v>
+        <v>0.0417343023927944</v>
       </c>
       <c r="EM2" t="n">
-        <v>0.0240564819850335</v>
+        <v>-0.00145577258648795</v>
       </c>
       <c r="EN2" t="n">
-        <v>0.0612932062753766</v>
+        <v>0.0104602450626872</v>
       </c>
       <c r="EO2" t="n">
-        <v>0.0424098493508203</v>
+        <v>0.0181627895729295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>